<commit_message>
HKD: add extrapolation in 6M curve to meet contribution problems, monitor refresh
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_MxContributor.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_MxContributor.xlsx
@@ -1099,112 +1099,110 @@
   <volType type="realTimeData">
     <main first="pldatasource.rtgetrtdserver">
       <tp>
-        <v>1.3400490860000001</v>
+        <v>1.55</v>
         <stp/>
         <stp>_x000C_HKD6M18X24F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T55" s="1"/>
       </tp>
       <tp>
-        <v>0.94436727499999995</v>
+        <v>1.210061871</v>
         <stp/>
         <stp>_x000C_HKD6M12X18F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T54" s="1"/>
       </tp>
       <tp>
-        <v>1.3400490860000001</v>
+        <v>1.55</v>
         <stp/>
         <stp>_x000C_HKD6M18X24F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U55" s="1"/>
       </tp>
       <tp>
-        <v>0.94436727499999995</v>
+        <v>1.210061871</v>
         <stp/>
         <stp>_x000C_HKD6M12X18F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U54" s="1"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>0.48635642299999998</v>
+      <tp>
+        <v>0.49</v>
         <stp/>
         <stp xml:space="preserve">
 HKD6M2X8F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T49" s="1"/>
       </tp>
       <tp>
-        <v>0.52133664199999996</v>
+        <v>0.51197530999999996</v>
         <stp/>
         <stp xml:space="preserve">
 HKD6M3X9F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T50" s="1"/>
       </tp>
       <tp>
-        <v>0.52133664199999996</v>
+        <v>0.51197530999999996</v>
         <stp/>
         <stp xml:space="preserve">
 HKD6M3X9F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U50" s="1"/>
       </tp>
       <tp>
-        <v>0.76</v>
+        <v>1.17</v>
         <stp/>
         <stp xml:space="preserve">	HKDSTD3Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U12" s="1"/>
       </tp>
       <tp>
-        <v>0.76</v>
+        <v>0.89</v>
         <stp/>
         <stp xml:space="preserve">	HKDSTD2Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U11" s="1"/>
       </tp>
       <tp>
-        <v>2.1</v>
+        <v>2.23</v>
         <stp/>
         <stp xml:space="preserve">	HKDSTD7Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U15" s="1"/>
       </tp>
       <tp>
-        <v>1.51</v>
+        <v>1.83</v>
         <stp/>
         <stp xml:space="preserve">	HKDSTD5Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U14" s="1"/>
       </tp>
       <tp>
-        <v>1.1200000000000001</v>
+        <v>1.55</v>
         <stp/>
         <stp xml:space="preserve">	HKDSTD4Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U13" s="1"/>
       </tp>
       <tp>
-        <v>0.48635642299999998</v>
+        <v>0.49</v>
         <stp/>
         <stp xml:space="preserve">
 HKD6M2X8F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U49" s="1"/>
       </tp>
       <tp>
-        <v>0.86356999999999995</v>
+        <v>0.84</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD1YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T10" s="1"/>
       </tp>
       <tp>
-        <v>0.47</v>
+        <v>0.46</v>
         <stp/>
         <stp xml:space="preserve">
 HKD3M6X9F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T27" s="1"/>
       </tp>
       <tp>
-        <v>0.47</v>
+        <v>0.46</v>
         <stp/>
         <stp xml:space="preserve">
 HKD3M6X9F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U27" s="1"/>
       </tp>
       <tp>
-        <v>0.86356999999999995</v>
+        <v>0.84</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD1YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
@@ -1218,28 +1216,28 @@
         <tr r="U26" s="1"/>
       </tp>
       <tp>
-        <v>0.4</v>
+        <v>0.38</v>
         <stp/>
         <stp xml:space="preserve">
 HKD3M1X4F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T25" s="1"/>
       </tp>
       <tp>
-        <v>0.13331000000000001</v>
+        <v>0.105</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD1WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U5" s="1"/>
       </tp>
       <tp>
-        <v>0.4</v>
+        <v>0.38</v>
         <stp/>
         <stp xml:space="preserve">
 HKD3M1X4F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U25" s="1"/>
       </tp>
       <tp>
-        <v>0.13331000000000001</v>
+        <v>0.105</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD1WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
@@ -1253,7 +1251,7 @@
         <tr r="T26" s="1"/>
       </tp>
       <tp>
-        <v>0.48933427000000002</v>
+        <v>0.47788269300000003</v>
         <stp/>
         <stp xml:space="preserve">
 HKD6M1X7F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
@@ -1358,42 +1356,42 @@
         <tr r="U87" s="1"/>
       </tp>
       <tp>
-        <v>0.48933427000000002</v>
+        <v>0.47788269300000003</v>
         <stp/>
         <stp xml:space="preserve">
 HKD6M1X7F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T48" s="1"/>
       </tp>
       <tp>
-        <v>0.21143000000000001</v>
+        <v>0.23080000000000001</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD1MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T6" s="1"/>
       </tp>
       <tp>
-        <v>0.37929000000000002</v>
+        <v>0.37429000000000001</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD3MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T8" s="1"/>
       </tp>
       <tp>
-        <v>0.31286000000000003</v>
+        <v>0.31219000000000002</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD2MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T7" s="1"/>
       </tp>
       <tp>
-        <v>0.54857</v>
+        <v>0.53571000000000002</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD6MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T9" s="1"/>
       </tp>
       <tp>
-        <v>6.8570000000000006E-2</v>
+        <v>5.4980000000000001E-2</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTDOND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
@@ -1402,35 +1400,35 @@
     </main>
     <main first="pldatasource.rtgetrtdserver">
       <tp>
-        <v>6.8570000000000006E-2</v>
+        <v>5.4980000000000001E-2</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTDOND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T4" s="1"/>
       </tp>
       <tp>
-        <v>0.21143000000000001</v>
+        <v>0.23080000000000001</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD1MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U6" s="1"/>
       </tp>
       <tp>
-        <v>0.37929000000000002</v>
+        <v>0.37429000000000001</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD3MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U8" s="1"/>
       </tp>
       <tp>
-        <v>0.31286000000000003</v>
+        <v>0.31219000000000002</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD2MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U7" s="1"/>
       </tp>
       <tp>
-        <v>0.54857</v>
+        <v>0.53571000000000002</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD6MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
@@ -1439,31 +1437,31 @@
     </main>
     <main first="pldatasource.rtgetrtdserver">
       <tp>
-        <v>0.76</v>
+        <v>0.89</v>
         <stp/>
         <stp xml:space="preserve">	HKDSTD2Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T11" s="1"/>
       </tp>
       <tp>
-        <v>0.76</v>
+        <v>1.17</v>
         <stp/>
         <stp xml:space="preserve">	HKDSTD3Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T12" s="1"/>
       </tp>
       <tp>
-        <v>1.1200000000000001</v>
+        <v>1.55</v>
         <stp/>
         <stp xml:space="preserve">	HKDSTD4Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T13" s="1"/>
       </tp>
       <tp>
-        <v>1.51</v>
+        <v>1.83</v>
         <stp/>
         <stp xml:space="preserve">	HKDSTD5Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T14" s="1"/>
       </tp>
       <tp>
-        <v>2.1</v>
+        <v>2.23</v>
         <stp/>
         <stp xml:space="preserve">	HKDSTD7Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T15" s="1"/>
@@ -1557,109 +1555,109 @@
     </main>
     <main first="pldatasource.rtgetrtdserver">
       <tp>
-        <v>0.40085707599999998</v>
+        <v>0.47598553100000002</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M12Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U78" s="1"/>
       </tp>
       <tp>
-        <v>0.39892309799999998</v>
+        <v>0.472755539</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M10Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U77" s="1"/>
       </tp>
       <tp>
-        <v>0.40264071400000001</v>
+        <v>0.47921625899999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M15Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U79" s="1"/>
       </tp>
       <tp>
-        <v>0.54782110799999995</v>
+        <v>0.66687071399999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD6MOND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T39" s="1"/>
       </tp>
       <tp>
-        <v>0.54784577499999998</v>
+        <v>0.66650554900000003</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M1WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T40" s="1"/>
       </tp>
       <tp>
-        <v>0.547940345</v>
+        <v>0.66195121499999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M1MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T42" s="1"/>
       </tp>
       <tp>
-        <v>0.54787455500000004</v>
+        <v>0.66580369100000003</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M2WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T41" s="1"/>
       </tp>
       <tp>
-        <v>0.54807195799999997</v>
+        <v>0.65108102899999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M2MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T43" s="1"/>
       </tp>
       <tp>
-        <v>0.54819126900000004</v>
+        <v>0.63181966199999995</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M3MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T44" s="1"/>
       </tp>
       <tp>
-        <v>0.54832707800000002</v>
+        <v>0.60396094</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M4MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T45" s="1"/>
       </tp>
       <tp>
-        <v>0.54844646200000002</v>
+        <v>0.57293082699999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M5MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T46" s="1"/>
       </tp>
       <tp>
-        <v>0.54290490199999997</v>
+        <v>0.53278898900000005</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M6MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T47" s="1"/>
       </tp>
       <tp>
-        <v>0.75574468299999997</v>
+        <v>0.885196659</v>
         <stp/>
         <stp>_x0008_HKD3M2Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U30" s="1"/>
       </tp>
       <tp>
-        <v>1.2084407859999999</v>
+        <v>1.348199003</v>
         <stp/>
         <stp>_x0008_HKD3M3Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U31" s="1"/>
       </tp>
       <tp>
-        <v>0.454087083</v>
+        <v>0.47234877400000003</v>
         <stp/>
         <stp>_x0008_HKD3M1Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U28" s="1"/>
       </tp>
       <tp>
-        <v>2.4158700450000001</v>
+        <v>2.1772487389999999</v>
         <stp/>
         <stp>_x0008_HKD3M7Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U34" s="1"/>
       </tp>
       <tp>
-        <v>1.6282329550000001</v>
+        <v>1.667477842</v>
         <stp/>
         <stp>_x0008_HKD3M4Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U32" s="1"/>
       </tp>
       <tp>
-        <v>1.956595831</v>
+        <v>1.887251314</v>
         <stp/>
         <stp>_x0008_HKD3M5Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U33" s="1"/>
@@ -1667,73 +1665,73 @@
     </main>
     <main first="pldatasource.rtgetrtdserver">
       <tp>
-        <v>2.9776409780000002</v>
+        <v>2.5486250909999999</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M12Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U36" s="1"/>
       </tp>
       <tp>
-        <v>2.808223022</v>
+        <v>2.43838577</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M10Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U35" s="1"/>
       </tp>
       <tp>
-        <v>3.068802823</v>
+        <v>2.648944073</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M15Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U37" s="1"/>
       </tp>
       <tp>
-        <v>0.35379251</v>
+        <v>0.395449728</v>
         <stp/>
         <stp>_x0008_HKD1M2Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U72" s="1"/>
       </tp>
       <tp>
-        <v>0.37220064899999999</v>
+        <v>0.42727208700000002</v>
         <stp/>
         <stp>_x0008_HKD1M3Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U73" s="1"/>
       </tp>
       <tp>
-        <v>0.21003202200000001</v>
+        <v>0.210032831</v>
         <stp/>
         <stp>_x0008_HKD1M3M=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U68" s="1"/>
       </tp>
       <tp>
-        <v>0.30017509199999998</v>
+        <v>0.34011009800000003</v>
         <stp/>
         <stp>_x0008_HKD1M1Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U71" s="1"/>
       </tp>
       <tp>
-        <v>0.24007155599999999</v>
+        <v>0.23008063200000001</v>
         <stp/>
         <stp>_x0008_HKD1M6M=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U69" s="1"/>
       </tp>
       <tp>
-        <v>0.39392157900000002</v>
+        <v>0.46435295700000001</v>
         <stp/>
         <stp>_x0008_HKD1M7Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U76" s="1"/>
       </tp>
       <tp>
-        <v>0.38158660700000002</v>
+        <v>0.44341164100000002</v>
         <stp/>
         <stp>_x0008_HKD1M4Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U74" s="1"/>
       </tp>
       <tp>
-        <v>0.38727832099999998</v>
+        <v>0.45314568599999999</v>
         <stp/>
         <stp>_x0008_HKD1M5Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U75" s="1"/>
       </tp>
       <tp>
-        <v>0.27011614900000003</v>
+        <v>0.25012948800000001</v>
         <stp/>
         <stp>_x0008_HKD1M9M=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U70" s="1"/>
@@ -1741,103 +1739,105 @@
     </main>
     <main first="pldatasource.rtgetrtdserver">
       <tp>
-        <v>0.35969663000000002</v>
+        <v>0.36853276200000001</v>
         <stp/>
         <stp xml:space="preserve">	HKD3MOND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T20" s="1"/>
       </tp>
       <tp>
-        <v>0.35981982800000001</v>
+        <v>0.36857559099999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M1WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T21" s="1"/>
       </tp>
       <tp>
-        <v>0.36185674000000001</v>
+        <v>0.369222049</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M1MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T23" s="1"/>
       </tp>
       <tp>
-        <v>0.36017699399999997</v>
+        <v>0.3686856</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M2WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T22" s="1"/>
       </tp>
       <tp>
-        <v>0.37929000000000002</v>
+        <v>0.37429000000000001</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M3MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T24" s="1"/>
       </tp>
       <tp>
-        <v>1.0130642990000001</v>
+        <v>1.0486416629999999</v>
         <stp/>
         <stp>_x0008_HKD6M3Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U56" s="1"/>
       </tp>
       <tp>
-        <v>1.195952914</v>
+        <v>1.2451725149999999</v>
         <stp/>
         <stp>_x0008_HKD6M7Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U59" s="1"/>
       </tp>
       <tp>
-        <v>1.0930755430000001</v>
+        <v>1.134443605</v>
         <stp/>
         <stp>_x0008_HKD6M4Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U57" s="1"/>
       </tp>
       <tp>
-        <v>1.1408896509999999</v>
+        <v>1.1860998060000001</v>
         <stp/>
         <stp>_x0008_HKD6M5Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U58" s="1"/>
       </tp>
       <tp>
-        <v>1.253187163</v>
+        <v>1.30656836</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M12Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U61" s="1"/>
       </tp>
       <tp>
-        <v>1.2372100479999999</v>
+        <v>1.2894010579999999</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M10Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U60" s="1"/>
       </tp>
       <tp>
-        <v>1.269216881</v>
+        <v>1.323734755</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M15Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U62" s="1"/>
       </tp>
       <tp>
-        <v>0.21360928400000001</v>
+        <v>0.23872455000000001</v>
         <stp/>
         <stp xml:space="preserve">	HKD1MOND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T64" s="1"/>
       </tp>
       <tp>
-        <v>0.21356529499999999</v>
+        <v>0.238575554</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M1WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T65" s="1"/>
       </tp>
       <tp>
-        <v>0.21356529499999999</v>
+        <v>0.238575554</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M1MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T67" s="1"/>
       </tp>
       <tp>
-        <v>0.21356529499999999</v>
+        <v>0.238575554</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M2WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T66" s="1"/>
       </tp>
-      <tp>
-        <v>2.95</v>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
+      <tp>
+        <v>2.84</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD15Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
@@ -1846,112 +1846,116 @@
     </main>
     <main first="pldatasource.rtgetrtdserver">
       <tp>
-        <v>1.0130642990000001</v>
+        <v>1.0486416629999999</v>
         <stp/>
         <stp>_x0008_HKD6M3Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T56" s="1"/>
       </tp>
       <tp>
-        <v>1.1408896509999999</v>
+        <v>1.1860998060000001</v>
         <stp/>
         <stp>_x0008_HKD6M5Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T58" s="1"/>
       </tp>
       <tp>
-        <v>1.0930755430000001</v>
+        <v>1.134443605</v>
         <stp/>
         <stp>_x0008_HKD6M4Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T57" s="1"/>
       </tp>
       <tp>
-        <v>1.195952914</v>
+        <v>1.2451725149999999</v>
         <stp/>
         <stp>_x0008_HKD6M7Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T59" s="1"/>
       </tp>
-      <tp>
-        <v>2.95</v>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
+      <tp>
+        <v>2.84</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD15Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U18" s="1"/>
       </tp>
       <tp>
-        <v>2.82</v>
+        <v>2.73</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD12Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U17" s="1"/>
       </tp>
       <tp>
-        <v>0.57588163599999997</v>
+        <v>0.67248073200000003</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M18M=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T29" s="1"/>
       </tp>
       <tp>
-        <v>2.63</v>
+        <v>2.58</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD10Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T16" s="1"/>
       </tp>
       <tp>
-        <v>0.30017509199999998</v>
+        <v>0.34011009800000003</v>
         <stp/>
         <stp>_x0008_HKD1M1Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T71" s="1"/>
       </tp>
       <tp>
-        <v>0.21003202200000001</v>
+        <v>0.210032831</v>
         <stp/>
         <stp>_x0008_HKD1M3M=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T68" s="1"/>
       </tp>
       <tp>
-        <v>0.37220064899999999</v>
+        <v>0.42727208700000002</v>
         <stp/>
         <stp>_x0008_HKD1M3Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T73" s="1"/>
       </tp>
       <tp>
-        <v>0.35379251</v>
+        <v>0.395449728</v>
         <stp/>
         <stp>_x0008_HKD1M2Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T72" s="1"/>
       </tp>
       <tp>
-        <v>0.38727832099999998</v>
+        <v>0.45314568599999999</v>
         <stp/>
         <stp>_x0008_HKD1M5Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T75" s="1"/>
       </tp>
       <tp>
-        <v>0.38158660700000002</v>
+        <v>0.44341164100000002</v>
         <stp/>
         <stp>_x0008_HKD1M4Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T74" s="1"/>
       </tp>
       <tp>
-        <v>0.39392157900000002</v>
+        <v>0.46435295700000001</v>
         <stp/>
         <stp>_x0008_HKD1M7Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T76" s="1"/>
       </tp>
       <tp>
-        <v>0.24007155599999999</v>
+        <v>0.23008063200000001</v>
         <stp/>
         <stp>_x0008_HKD1M6M=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T69" s="1"/>
       </tp>
       <tp>
-        <v>0.27011614900000003</v>
+        <v>0.25012948800000001</v>
         <stp/>
         <stp>_x0008_HKD1M9M=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T70" s="1"/>
       </tp>
-      <tp>
-        <v>2.63</v>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
+      <tp>
+        <v>2.58</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD10Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
@@ -1960,212 +1964,212 @@
     </main>
     <main first="pldatasource.rtgetrtdserver">
       <tp>
-        <v>2.82</v>
+        <v>2.73</v>
         <stp/>
         <stp xml:space="preserve">
 HKDSTD12Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T17" s="1"/>
       </tp>
       <tp>
-        <v>0.454087083</v>
+        <v>0.47234877400000003</v>
         <stp/>
         <stp>_x0008_HKD3M1Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T28" s="1"/>
       </tp>
       <tp>
-        <v>1.2084407859999999</v>
+        <v>1.348199003</v>
         <stp/>
         <stp>_x0008_HKD3M3Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T31" s="1"/>
       </tp>
       <tp>
-        <v>0.75574468299999997</v>
+        <v>0.885196659</v>
         <stp/>
         <stp>_x0008_HKD3M2Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T30" s="1"/>
       </tp>
       <tp>
-        <v>1.956595831</v>
+        <v>1.887251314</v>
         <stp/>
         <stp>_x0008_HKD3M5Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T33" s="1"/>
       </tp>
       <tp>
-        <v>1.6282329550000001</v>
+        <v>1.667477842</v>
         <stp/>
         <stp>_x0008_HKD3M4Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T32" s="1"/>
       </tp>
       <tp>
-        <v>2.4158700450000001</v>
+        <v>2.1772487389999999</v>
         <stp/>
         <stp>_x0008_HKD3M7Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T34" s="1"/>
       </tp>
       <tp>
-        <v>0.57588163599999997</v>
+        <v>0.67248073200000003</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M18M=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U29" s="1"/>
       </tp>
       <tp>
-        <v>2.808223022</v>
+        <v>2.43838577</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M10Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T35" s="1"/>
       </tp>
       <tp>
-        <v>2.9776409780000002</v>
+        <v>2.5486250909999999</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M12Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T36" s="1"/>
       </tp>
       <tp>
-        <v>3.068802823</v>
+        <v>2.648944073</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M15Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T37" s="1"/>
       </tp>
       <tp>
-        <v>0.54782110799999995</v>
+        <v>0.66687071399999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD6MOND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U39" s="1"/>
       </tp>
       <tp>
-        <v>0.54784577499999998</v>
+        <v>0.66650554900000003</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M1WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U40" s="1"/>
       </tp>
       <tp>
-        <v>0.547940345</v>
+        <v>0.66195121499999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M1MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U42" s="1"/>
       </tp>
       <tp>
-        <v>0.54787455500000004</v>
+        <v>0.66580369100000003</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M2WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U41" s="1"/>
       </tp>
       <tp>
-        <v>0.54807195799999997</v>
+        <v>0.65108102899999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M2MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U43" s="1"/>
       </tp>
       <tp>
-        <v>0.54819126900000004</v>
+        <v>0.63181966199999995</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M3MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U44" s="1"/>
       </tp>
       <tp>
-        <v>0.54832707800000002</v>
+        <v>0.60396094</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M4MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U45" s="1"/>
       </tp>
       <tp>
-        <v>0.54844646200000002</v>
+        <v>0.57293082699999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M5MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U46" s="1"/>
       </tp>
       <tp>
-        <v>0.54290490199999997</v>
+        <v>0.53278898900000005</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M6MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U47" s="1"/>
       </tp>
       <tp>
-        <v>0.39892309799999998</v>
+        <v>0.472755539</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M10Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T77" s="1"/>
       </tp>
       <tp>
-        <v>0.40085707599999998</v>
+        <v>0.47598553100000002</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M12Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T78" s="1"/>
       </tp>
       <tp>
-        <v>0.40264071400000001</v>
+        <v>0.47921625899999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M15Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T79" s="1"/>
       </tp>
       <tp>
-        <v>0.21360928400000001</v>
+        <v>0.23872455000000001</v>
         <stp/>
         <stp xml:space="preserve">	HKD1MOND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U64" s="1"/>
       </tp>
       <tp>
-        <v>0.21356529499999999</v>
+        <v>0.238575554</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M1WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U65" s="1"/>
       </tp>
       <tp>
-        <v>0.21356529499999999</v>
+        <v>0.238575554</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M1MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U67" s="1"/>
       </tp>
       <tp>
-        <v>0.21356529499999999</v>
+        <v>0.238575554</v>
         <stp/>
         <stp xml:space="preserve">	HKD1M2WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U66" s="1"/>
       </tp>
       <tp>
-        <v>1.2372100479999999</v>
+        <v>1.2894010579999999</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M10Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T60" s="1"/>
       </tp>
       <tp>
-        <v>1.253187163</v>
+        <v>1.30656836</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M12Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T61" s="1"/>
       </tp>
       <tp>
-        <v>1.269216881</v>
+        <v>1.323734755</v>
         <stp/>
         <stp xml:space="preserve">	HKD6M15Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T62" s="1"/>
       </tp>
       <tp>
-        <v>0.35969663000000002</v>
+        <v>0.36853276200000001</v>
         <stp/>
         <stp xml:space="preserve">	HKD3MOND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U20" s="1"/>
       </tp>
       <tp>
-        <v>0.35981982800000001</v>
+        <v>0.36857559099999998</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M1WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U21" s="1"/>
       </tp>
       <tp>
-        <v>0.36185674000000001</v>
+        <v>0.369222049</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M1MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U23" s="1"/>
       </tp>
       <tp>
-        <v>0.36017699399999997</v>
+        <v>0.3686856</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M2WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U22" s="1"/>
       </tp>
       <tp>
-        <v>0.37929000000000002</v>
+        <v>0.37429000000000001</v>
         <stp/>
         <stp xml:space="preserve">	HKD3M3MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U24" s="1"/>
@@ -2221,37 +2225,37 @@
         <tr r="T97" s="1"/>
       </tp>
       <tp>
-        <v>0.54359215800000005</v>
+        <v>0.55549872099999997</v>
         <stp/>
         <stp>_x000B_HKD6M4X10F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U51" s="1"/>
       </tp>
       <tp>
-        <v>0.56194412699999996</v>
+        <v>0.59318432300000001</v>
         <stp/>
         <stp>_x000B_HKD6M5X11F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U52" s="1"/>
       </tp>
       <tp>
-        <v>0.59967255399999997</v>
+        <v>0.63192839199999995</v>
         <stp/>
         <stp>_x000B_HKD6M6X12F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T53" s="1"/>
       </tp>
       <tp>
-        <v>0.59967255399999997</v>
+        <v>0.63192839199999995</v>
         <stp/>
         <stp>_x000B_HKD6M6X12F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="U53" s="1"/>
       </tp>
       <tp>
-        <v>0.56194412699999996</v>
+        <v>0.59318432300000001</v>
         <stp/>
         <stp>_x000B_HKD6M5X11F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T52" s="1"/>
       </tp>
       <tp>
-        <v>0.54359215800000005</v>
+        <v>0.55549872099999997</v>
         <stp/>
         <stp>_x000B_HKD6M4X10F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="T51" s="1"/>
@@ -2284,44 +2288,44 @@
       <sheetData sheetId="0">
         <row r="22">
           <cell r="D22">
-            <v>2</v>
+            <v>4</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="6">
           <cell r="V6">
-            <v>5.6610000000000001E-2</v>
+            <v>5.4980000000000001E-2</v>
           </cell>
         </row>
         <row r="7">
           <cell r="V7">
-            <v>0.12714</v>
+            <v>0.105</v>
           </cell>
         </row>
         <row r="9">
           <cell r="V9">
-            <v>0.20571</v>
+            <v>0.23080000000000001</v>
           </cell>
         </row>
         <row r="10">
           <cell r="V10">
-            <v>0.30286000000000002</v>
+            <v>0.31219000000000002</v>
           </cell>
         </row>
         <row r="11">
           <cell r="V11">
-            <v>0.37142999999999998</v>
+            <v>0.37429000000000001</v>
           </cell>
         </row>
         <row r="12">
           <cell r="V12">
-            <v>0.54857</v>
+            <v>0.53571000000000002</v>
           </cell>
         </row>
         <row r="14">
           <cell r="V14">
-            <v>0.86285999999999996</v>
+            <v>0.84</v>
           </cell>
         </row>
       </sheetData>
@@ -2329,42 +2333,42 @@
       <sheetData sheetId="3">
         <row r="8">
           <cell r="Q8">
-            <v>0.05</v>
+            <v>0.06</v>
           </cell>
         </row>
         <row r="9">
           <cell r="Q9">
-            <v>6.9999999999999993E-2</v>
+            <v>0.06</v>
           </cell>
         </row>
         <row r="10">
           <cell r="Q10">
-            <v>9.0000000000000011E-2</v>
+            <v>6.9999999999999993E-2</v>
           </cell>
         </row>
         <row r="11">
           <cell r="Q11">
-            <v>0.12000000000000001</v>
+            <v>0.1</v>
           </cell>
         </row>
         <row r="12">
           <cell r="Q12">
-            <v>0.1</v>
+            <v>0.11</v>
           </cell>
         </row>
         <row r="13">
           <cell r="Q13">
-            <v>0.11</v>
+            <v>0.12000000000000001</v>
           </cell>
         </row>
         <row r="16">
           <cell r="Q16">
-            <v>0.16999999999999998</v>
+            <v>0.13</v>
           </cell>
         </row>
         <row r="19">
           <cell r="Q19">
-            <v>0.2</v>
+            <v>0.15000000000000002</v>
           </cell>
         </row>
         <row r="22">
@@ -2384,7 +2388,7 @@
       <sheetData sheetId="6">
         <row r="22">
           <cell r="D22" t="str">
-            <v>V5</v>
+            <v>J6</v>
           </cell>
         </row>
       </sheetData>
@@ -2392,37 +2396,37 @@
       <sheetData sheetId="8">
         <row r="10">
           <cell r="Q10">
-            <v>0.72</v>
+            <v>0.8899999999999999</v>
           </cell>
         </row>
         <row r="11">
           <cell r="S11">
-            <v>0.76</v>
+            <v>1.17</v>
           </cell>
         </row>
         <row r="12">
           <cell r="S12">
-            <v>1.1200000000000001</v>
+            <v>1.55</v>
           </cell>
         </row>
         <row r="13">
           <cell r="S13">
-            <v>1.51</v>
+            <v>1.83</v>
           </cell>
         </row>
         <row r="15">
           <cell r="S15">
-            <v>2.0999999999999996</v>
+            <v>2.23</v>
           </cell>
         </row>
         <row r="18">
           <cell r="S18">
-            <v>2.63</v>
+            <v>2.58</v>
           </cell>
         </row>
         <row r="20">
           <cell r="S20">
-            <v>2.8200000000000003</v>
+            <v>2.73</v>
           </cell>
         </row>
         <row r="22">
@@ -2432,7 +2436,7 @@
         </row>
         <row r="23">
           <cell r="S23">
-            <v>2.95</v>
+            <v>2.84</v>
           </cell>
         </row>
       </sheetData>
@@ -2746,8 +2750,8 @@
   <dimension ref="A1:U118"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
+      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2756,19 +2760,20 @@
     <col min="2" max="2" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="4" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="25.140625" style="4" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="9.42578125" style="4" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="30.28515625" style="4" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="25.140625" style="4" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="7" style="4" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.42578125" style="6" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="4" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="25.140625" style="4" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="9.42578125" style="4" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="30.28515625" style="4" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="25.140625" style="4" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="7" style="4" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.42578125" style="6" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="22.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="19.140625" style="6" customWidth="1"/>
     <col min="14" max="16" width="19.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="8.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="70.5703125" style="4" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="21" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="70.5703125" style="4" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="11.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -2783,17 +2788,17 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4">
         <f>[1]!TriggerCounter</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R1" s="7"/>
       <c r="S1" s="8">
-        <v>41736.443773148145</v>
+        <v>41918.580208333333</v>
       </c>
     </row>
     <row r="2" spans="2:21" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2923,11 +2928,11 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="19">
         <f>[1]Hibor!$V$6</f>
-        <v>5.6610000000000001E-2</v>
+        <v>5.4980000000000001E-2</v>
       </c>
       <c r="R4" s="19">
         <f t="shared" ref="R4:R18" si="0">Q4</f>
-        <v>5.6610000000000001E-2</v>
+        <v>5.4980000000000001E-2</v>
       </c>
       <c r="S4" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K4),_xll.RtContribute(SourceAlias,$L4,Fields,Q4:R4,"SCOPE:SERVER"),"--")</f>
@@ -2935,11 +2940,11 @@
       </c>
       <c r="T4" s="19">
         <f>IF($K4,ABS(_xll.RtGet(SourceAlias,$L4,Q$2)-Q4),0)</f>
-        <v>1.1960000000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="U4" s="19">
         <f>IF($K4,ABS(_xll.RtGet(SourceAlias,$L4,R$2)-R4),0)</f>
-        <v>1.1960000000000005E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2982,11 +2987,11 @@
       <c r="P5" s="18"/>
       <c r="Q5" s="19">
         <f>[1]Hibor!$V$7</f>
-        <v>0.12714</v>
+        <v>0.105</v>
       </c>
       <c r="R5" s="19">
         <f t="shared" si="0"/>
-        <v>0.12714</v>
+        <v>0.105</v>
       </c>
       <c r="S5" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K5),_xll.RtContribute(SourceAlias,$L5,Fields,Q5:R5,"SCOPE:SERVER"),"--")</f>
@@ -2994,11 +2999,11 @@
       </c>
       <c r="T5" s="19">
         <f>IF($K5,ABS(_xll.RtGet(SourceAlias,$L5,Q$2)-Q5),0)</f>
-        <v>6.1700000000000088E-3</v>
+        <v>0</v>
       </c>
       <c r="U5" s="19">
         <f>IF($K5,ABS(_xll.RtGet(SourceAlias,$L5,R$2)-R5),0)</f>
-        <v>6.1700000000000088E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3041,11 +3046,11 @@
       <c r="P6" s="18"/>
       <c r="Q6" s="19">
         <f>[1]Hibor!$V$9</f>
-        <v>0.20571</v>
+        <v>0.23080000000000001</v>
       </c>
       <c r="R6" s="19">
         <f t="shared" si="0"/>
-        <v>0.20571</v>
+        <v>0.23080000000000001</v>
       </c>
       <c r="S6" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K6),_xll.RtContribute(SourceAlias,$L6,Fields,Q6:R6,"SCOPE:SERVER"),"--")</f>
@@ -3053,11 +3058,11 @@
       </c>
       <c r="T6" s="19">
         <f>IF($K6,ABS(_xll.RtGet(SourceAlias,$L6,Q$2)-Q6),0)</f>
-        <v>5.7200000000000029E-3</v>
+        <v>0</v>
       </c>
       <c r="U6" s="19">
         <f>IF($K6,ABS(_xll.RtGet(SourceAlias,$L6,R$2)-R6),0)</f>
-        <v>5.7200000000000029E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3100,11 +3105,11 @@
       <c r="P7" s="18"/>
       <c r="Q7" s="19">
         <f>[1]Hibor!$V$10</f>
-        <v>0.30286000000000002</v>
+        <v>0.31219000000000002</v>
       </c>
       <c r="R7" s="19">
         <f t="shared" si="0"/>
-        <v>0.30286000000000002</v>
+        <v>0.31219000000000002</v>
       </c>
       <c r="S7" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K7),_xll.RtContribute(SourceAlias,$L7,Fields,Q7:R7,"SCOPE:SERVER"),"--")</f>
@@ -3112,11 +3117,11 @@
       </c>
       <c r="T7" s="19">
         <f>IF($K7,ABS(_xll.RtGet(SourceAlias,$L7,Q$2)-Q7),0)</f>
-        <v>1.0000000000000009E-2</v>
+        <v>0</v>
       </c>
       <c r="U7" s="19">
         <f>IF($K7,ABS(_xll.RtGet(SourceAlias,$L7,R$2)-R7),0)</f>
-        <v>1.0000000000000009E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3159,11 +3164,11 @@
       <c r="P8" s="18"/>
       <c r="Q8" s="19">
         <f>[1]Hibor!$V$11</f>
-        <v>0.37142999999999998</v>
+        <v>0.37429000000000001</v>
       </c>
       <c r="R8" s="19">
         <f t="shared" si="0"/>
-        <v>0.37142999999999998</v>
+        <v>0.37429000000000001</v>
       </c>
       <c r="S8" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K8),_xll.RtContribute(SourceAlias,$L8,Fields,Q8:R8,"SCOPE:SERVER"),"--")</f>
@@ -3171,11 +3176,11 @@
       </c>
       <c r="T8" s="19">
         <f>IF($K8,ABS(_xll.RtGet(SourceAlias,$L8,Q$2)-Q8),0)</f>
-        <v>7.8600000000000336E-3</v>
+        <v>0</v>
       </c>
       <c r="U8" s="19">
         <f>IF($K8,ABS(_xll.RtGet(SourceAlias,$L8,R$2)-R8),0)</f>
-        <v>7.8600000000000336E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3218,11 +3223,11 @@
       <c r="P9" s="18"/>
       <c r="Q9" s="19">
         <f>[1]Hibor!$V$12</f>
-        <v>0.54857</v>
+        <v>0.53571000000000002</v>
       </c>
       <c r="R9" s="19">
         <f t="shared" si="0"/>
-        <v>0.54857</v>
+        <v>0.53571000000000002</v>
       </c>
       <c r="S9" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K9),_xll.RtContribute(SourceAlias,$L9,Fields,Q9:R9,"SCOPE:SERVER"),"--")</f>
@@ -3277,11 +3282,11 @@
       <c r="P10" s="18"/>
       <c r="Q10" s="19">
         <f>[1]Hibor!$V$14</f>
-        <v>0.86285999999999996</v>
+        <v>0.84</v>
       </c>
       <c r="R10" s="19">
         <f t="shared" si="0"/>
-        <v>0.86285999999999996</v>
+        <v>0.84</v>
       </c>
       <c r="S10" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K10),_xll.RtContribute(SourceAlias,$L10,Fields,Q10:R10,"SCOPE:SERVER"),"--")</f>
@@ -3289,11 +3294,11 @@
       </c>
       <c r="T10" s="19">
         <f>IF($K10,ABS(_xll.RtGet(SourceAlias,$L10,Q$2)-Q10),0)</f>
-        <v>7.0999999999998842E-4</v>
+        <v>0</v>
       </c>
       <c r="U10" s="19">
         <f>IF($K10,ABS(_xll.RtGet(SourceAlias,$L10,R$2)-R10),0)</f>
-        <v>7.0999999999998842E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3336,11 +3341,11 @@
       <c r="P11" s="18"/>
       <c r="Q11" s="19">
         <f>[1]Swap3M!$Q$10</f>
-        <v>0.72</v>
+        <v>0.8899999999999999</v>
       </c>
       <c r="R11" s="19">
         <f t="shared" si="0"/>
-        <v>0.72</v>
+        <v>0.8899999999999999</v>
       </c>
       <c r="S11" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K11),_xll.RtContribute(SourceAlias,$L11,Fields,Q11:R11,"SCOPE:SERVER"),"--")</f>
@@ -3348,11 +3353,11 @@
       </c>
       <c r="T11" s="19">
         <f>IF($K11,ABS(_xll.RtGet(SourceAlias,$L11,Q$2)-Q11),0)</f>
-        <v>4.0000000000000036E-2</v>
+        <v>1.1102230246251565E-16</v>
       </c>
       <c r="U11" s="19">
         <f>IF($K11,ABS(_xll.RtGet(SourceAlias,$L11,R$2)-R11),0)</f>
-        <v>4.0000000000000036E-2</v>
+        <v>1.1102230246251565E-16</v>
       </c>
     </row>
     <row r="12" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3395,11 +3400,11 @@
       <c r="P12" s="18"/>
       <c r="Q12" s="19">
         <f>[1]Swap3M!$S$11</f>
-        <v>0.76</v>
+        <v>1.17</v>
       </c>
       <c r="R12" s="19">
         <f t="shared" si="0"/>
-        <v>0.76</v>
+        <v>1.17</v>
       </c>
       <c r="S12" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K12),_xll.RtContribute(SourceAlias,$L12,Fields,Q12:R12,"SCOPE:SERVER"),"--")</f>
@@ -3454,11 +3459,11 @@
       <c r="P13" s="18"/>
       <c r="Q13" s="19">
         <f>[1]Swap3M!$S$12</f>
-        <v>1.1200000000000001</v>
+        <v>1.55</v>
       </c>
       <c r="R13" s="19">
         <f t="shared" si="0"/>
-        <v>1.1200000000000001</v>
+        <v>1.55</v>
       </c>
       <c r="S13" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K13),_xll.RtContribute(SourceAlias,$L13,Fields,Q13:R13,"SCOPE:SERVER"),"--")</f>
@@ -3513,11 +3518,11 @@
       <c r="P14" s="18"/>
       <c r="Q14" s="19">
         <f>[1]Swap3M!$S$13</f>
-        <v>1.51</v>
+        <v>1.83</v>
       </c>
       <c r="R14" s="19">
         <f t="shared" si="0"/>
-        <v>1.51</v>
+        <v>1.83</v>
       </c>
       <c r="S14" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K14),_xll.RtContribute(SourceAlias,$L14,Fields,Q14:R14,"SCOPE:SERVER"),"--")</f>
@@ -3572,11 +3577,11 @@
       <c r="P15" s="18"/>
       <c r="Q15" s="19">
         <f>[1]Swap3M!$S$15</f>
-        <v>2.0999999999999996</v>
+        <v>2.23</v>
       </c>
       <c r="R15" s="19">
         <f t="shared" si="0"/>
-        <v>2.0999999999999996</v>
+        <v>2.23</v>
       </c>
       <c r="S15" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K15),_xll.RtContribute(SourceAlias,$L15,Fields,Q15:R15,"SCOPE:SERVER"),"--")</f>
@@ -3584,11 +3589,11 @@
       </c>
       <c r="T15" s="19">
         <f>IF($K15,ABS(_xll.RtGet(SourceAlias,$L15,Q$2)-Q15),0)</f>
-        <v>4.4408920985006262E-16</v>
+        <v>0</v>
       </c>
       <c r="U15" s="19">
         <f>IF($K15,ABS(_xll.RtGet(SourceAlias,$L15,R$2)-R15),0)</f>
-        <v>4.4408920985006262E-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3631,11 +3636,11 @@
       <c r="P16" s="18"/>
       <c r="Q16" s="19">
         <f>[1]Swap3M!$S$18</f>
-        <v>2.63</v>
+        <v>2.58</v>
       </c>
       <c r="R16" s="19">
         <f t="shared" si="0"/>
-        <v>2.63</v>
+        <v>2.58</v>
       </c>
       <c r="S16" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K16),_xll.RtContribute(SourceAlias,$L16,Fields,Q16:R16,"SCOPE:SERVER"),"--")</f>
@@ -3690,11 +3695,11 @@
       <c r="P17" s="18"/>
       <c r="Q17" s="19">
         <f>[1]Swap3M!$S$20</f>
-        <v>2.8200000000000003</v>
+        <v>2.73</v>
       </c>
       <c r="R17" s="19">
         <f t="shared" si="0"/>
-        <v>2.8200000000000003</v>
+        <v>2.73</v>
       </c>
       <c r="S17" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K17),_xll.RtContribute(SourceAlias,$L17,Fields,Q17:R17,"SCOPE:SERVER"),"--")</f>
@@ -3702,11 +3707,11 @@
       </c>
       <c r="T17" s="19">
         <f>IF($K17,ABS(_xll.RtGet(SourceAlias,$L17,Q$2)-Q17),0)</f>
-        <v>4.4408920985006262E-16</v>
+        <v>0</v>
       </c>
       <c r="U17" s="19">
         <f>IF($K17,ABS(_xll.RtGet(SourceAlias,$L17,R$2)-R17),0)</f>
-        <v>4.4408920985006262E-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3749,11 +3754,11 @@
       <c r="P18" s="18"/>
       <c r="Q18" s="19">
         <f>[1]Swap3M!$S$23</f>
-        <v>2.95</v>
+        <v>2.84</v>
       </c>
       <c r="R18" s="19">
         <f t="shared" si="0"/>
-        <v>2.95</v>
+        <v>2.84</v>
       </c>
       <c r="S18" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K18),_xll.RtContribute(SourceAlias,$L18,Fields,Q18:R18,"SCOPE:SERVER"),"--")</f>
@@ -3832,19 +3837,19 @@
       <c r="N20" s="47"/>
       <c r="O20" s="47">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J20)</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="P20" s="47">
         <f>_xll.qlCalendarAdvance(Calendar,O20,"1d",,TRUE)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="Q20" s="48">
         <f>(_xll.qlYieldTSDiscount($F$19,O20,TriggerCounter)/_xll.qlYieldTSDiscount($F$19,P20)-1)/_xll.qlDayCounterYearFraction(F20,O20,P20)*100</f>
-        <v>0.34432242800475077</v>
+        <v>0.37011576075718366</v>
       </c>
       <c r="R20" s="48">
         <f t="shared" ref="R20:R83" si="1">Q20</f>
-        <v>0.34432242800475077</v>
+        <v>0.37011576075718366</v>
       </c>
       <c r="S20" s="49" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K20),_xll.RtContribute(SourceAlias,$L20,Fields,Q20:R20,"SCOPE:SERVER"),"--")</f>
@@ -3852,11 +3857,11 @@
       </c>
       <c r="T20" s="48">
         <f>IF($K20,ABS(_xll.RtGet(SourceAlias,$L20,Q$2)-Q20),0)</f>
-        <v>1.5374201995249248E-2</v>
+        <v>1.5829987571836512E-3</v>
       </c>
       <c r="U20" s="50">
         <f>IF($K20,ABS(_xll.RtGet(SourceAlias,$L20,R$2)-R20),0)</f>
-        <v>1.5374201995249248E-2</v>
+        <v>1.5829987571836512E-3</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3897,19 +3902,19 @@
       <c r="N21" s="51"/>
       <c r="O21" s="51">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J21)</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="P21" s="51">
         <f>_xll.qlCalendarAdvance(Calendar,O21,B21)</f>
-        <v>41743</v>
+        <v>41925</v>
       </c>
       <c r="Q21" s="52">
         <f>(_xll.qlYieldTSDiscount($F$19,O21,TriggerCounter)/_xll.qlYieldTSDiscount($F$19,P21)-1)/_xll.qlDayCounterYearFraction(F21,O21,P21)*100</f>
-        <v>0.34448834136126455</v>
+        <v>0.37014970677538639</v>
       </c>
       <c r="R21" s="52">
         <f t="shared" si="1"/>
-        <v>0.34448834136126455</v>
+        <v>0.37014970677538639</v>
       </c>
       <c r="S21" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K21),_xll.RtContribute(SourceAlias,$L21,Fields,Q21:R21,"SCOPE:SERVER"),"--")</f>
@@ -3917,11 +3922,11 @@
       </c>
       <c r="T21" s="52">
         <f>IF($K21,ABS(_xll.RtGet(SourceAlias,$L21,Q$2)-Q21),0)</f>
-        <v>1.5331486638735459E-2</v>
+        <v>1.5741157753864088E-3</v>
       </c>
       <c r="U21" s="54">
         <f>IF($K21,ABS(_xll.RtGet(SourceAlias,$L21,R$2)-R21),0)</f>
-        <v>1.5331486638735459E-2</v>
+        <v>1.5741157753864088E-3</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3962,19 +3967,19 @@
       <c r="N22" s="51"/>
       <c r="O22" s="51">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J22)</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="P22" s="51">
         <f>_xll.qlCalendarAdvance(Calendar,O22,B22)</f>
-        <v>41751</v>
+        <v>41932</v>
       </c>
       <c r="Q22" s="52">
         <f>(_xll.qlYieldTSDiscount($F$19,O22,TriggerCounter)/_xll.qlYieldTSDiscount($F$19,P22)-1)/_xll.qlDayCounterYearFraction(F22,O22,P22)*100</f>
-        <v>0.34507400851444547</v>
+        <v>0.37023232785778265</v>
       </c>
       <c r="R22" s="52">
         <f t="shared" si="1"/>
-        <v>0.34507400851444547</v>
+        <v>0.37023232785778265</v>
       </c>
       <c r="S22" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K22),_xll.RtContribute(SourceAlias,$L22,Fields,Q22:R22,"SCOPE:SERVER"),"--")</f>
@@ -3982,11 +3987,11 @@
       </c>
       <c r="T22" s="52">
         <f>IF($K22,ABS(_xll.RtGet(SourceAlias,$L22,Q$2)-Q22),0)</f>
-        <v>1.5102985485554499E-2</v>
+        <v>1.5467278577826482E-3</v>
       </c>
       <c r="U22" s="54">
         <f>IF($K22,ABS(_xll.RtGet(SourceAlias,$L22,R$2)-R22),0)</f>
-        <v>1.5102985485554499E-2</v>
+        <v>1.5467278577826482E-3</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4027,19 +4032,19 @@
       <c r="N23" s="51"/>
       <c r="O23" s="51">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J23)</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="P23" s="51">
         <f>_xll.qlCalendarAdvance(Calendar,O23,B23,,TRUE)</f>
-        <v>41766</v>
+        <v>41949</v>
       </c>
       <c r="Q23" s="52">
         <f>(_xll.qlYieldTSDiscount($F$19,O23,TriggerCounter)/_xll.qlYieldTSDiscount($F$19,P23)-1)/_xll.qlDayCounterYearFraction(F23,O23,P23)*100</f>
-        <v>0.34729507858029346</v>
+        <v>0.37062590698552333</v>
       </c>
       <c r="R23" s="52">
         <f t="shared" si="1"/>
-        <v>0.34729507858029346</v>
+        <v>0.37062590698552333</v>
       </c>
       <c r="S23" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K23),_xll.RtContribute(SourceAlias,$L23,Fields,Q23:R23,"SCOPE:SERVER"),"--")</f>
@@ -4047,11 +4052,11 @@
       </c>
       <c r="T23" s="52">
         <f>IF($K23,ABS(_xll.RtGet(SourceAlias,$L23,Q$2)-Q23),0)</f>
-        <v>1.4561661419706551E-2</v>
+        <v>1.403857985523338E-3</v>
       </c>
       <c r="U23" s="54">
         <f>IF($K23,ABS(_xll.RtGet(SourceAlias,$L23,R$2)-R23),0)</f>
-        <v>1.4561661419706551E-2</v>
+        <v>1.403857985523338E-3</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4092,19 +4097,19 @@
       <c r="N24" s="55"/>
       <c r="O24" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J24)</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="P24" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,O24,B24,,TRUE)</f>
-        <v>41827</v>
+        <v>42010</v>
       </c>
       <c r="Q24" s="56">
         <f>(_xll.qlYieldTSDiscount($F$19,O24,TriggerCounter)/_xll.qlYieldTSDiscount($F$19,P24)-1)/_xll.qlDayCounterYearFraction(F24,O24,P24)*100</f>
-        <v>0.37142999997977483</v>
+        <v>0.37428999997795898</v>
       </c>
       <c r="R24" s="56">
         <f t="shared" si="1"/>
-        <v>0.37142999997977483</v>
+        <v>0.37428999997795898</v>
       </c>
       <c r="S24" s="57" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K24),_xll.RtContribute(SourceAlias,$L24,Fields,Q24:R24,"SCOPE:SERVER"),"--")</f>
@@ -4112,11 +4117,11 @@
       </c>
       <c r="T24" s="56">
         <f>IF($K24,ABS(_xll.RtGet(SourceAlias,$L24,Q$2)-Q24),0)</f>
-        <v>7.8600000202251885E-3</v>
+        <v>2.2041035663278308E-11</v>
       </c>
       <c r="U24" s="58">
         <f>IF($K24,ABS(_xll.RtGet(SourceAlias,$L24,R$2)-R24),0)</f>
-        <v>7.8600000202251885E-3</v>
+        <v>2.2041035663278308E-11</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4159,23 +4164,23 @@
       <c r="M25" s="47"/>
       <c r="N25" s="47">
         <f>_xll.qlInterestRateIndexFixingDate(H25,O25)</f>
-        <v>41766</v>
+        <v>41949</v>
       </c>
       <c r="O25" s="47">
         <f>_xll.qlCalendarAdvance(Calendar,$O$21,A25,,TRUE)</f>
-        <v>41766</v>
+        <v>41949</v>
       </c>
       <c r="P25" s="47">
         <f>_xll.qlInterestRateIndexMaturity(H25,O25)</f>
-        <v>41858</v>
+        <v>42041</v>
       </c>
       <c r="Q25" s="48">
         <f>_xll.qlIndexFixing(H25,N25,,TriggerCounter)*100</f>
-        <v>0.40000000030350541</v>
+        <v>0.37999999989853273</v>
       </c>
       <c r="R25" s="48">
         <f t="shared" si="1"/>
-        <v>0.40000000030350541</v>
+        <v>0.37999999989853273</v>
       </c>
       <c r="S25" s="49" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K25),_xll.RtContribute(SourceAlias,$L25,Fields,Q25:R25,"SCOPE:SERVER"),"--")</f>
@@ -4183,11 +4188,11 @@
       </c>
       <c r="T25" s="48">
         <f>IF($K25,ABS(_xll.RtGet(SourceAlias,$L25,Q$2)-Q25),0)</f>
-        <v>3.0350538748891154E-10</v>
+        <v>1.0146727902338171E-10</v>
       </c>
       <c r="U25" s="50">
         <f>IF($K25,ABS(_xll.RtGet(SourceAlias,$L25,R$2)-R25),0)</f>
-        <v>3.0350538748891154E-10</v>
+        <v>1.0146727902338171E-10</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4230,23 +4235,23 @@
       <c r="M26" s="51"/>
       <c r="N26" s="51">
         <f>_xll.qlInterestRateIndexFixingDate(H26,O26)</f>
-        <v>41827</v>
+        <v>42010</v>
       </c>
       <c r="O26" s="51">
         <f>_xll.qlCalendarAdvance(Calendar,$O$21,A26,,TRUE)</f>
-        <v>41827</v>
+        <v>42010</v>
       </c>
       <c r="P26" s="51">
         <f>_xll.qlInterestRateIndexMaturity(H26,O26)</f>
-        <v>41919</v>
+        <v>42101</v>
       </c>
       <c r="Q26" s="52">
         <f>_xll.qlIndexFixing(H26,N26,,TriggerCounter)*100</f>
-        <v>0.41000000000002501</v>
+        <v>0.41999999999998816</v>
       </c>
       <c r="R26" s="52">
         <f t="shared" si="1"/>
-        <v>0.41000000000002501</v>
+        <v>0.41999999999998816</v>
       </c>
       <c r="S26" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K26),_xll.RtContribute(SourceAlias,$L26,Fields,Q26:R26,"SCOPE:SERVER"),"--")</f>
@@ -4254,11 +4259,11 @@
       </c>
       <c r="T26" s="52">
         <f>IF($K26,ABS(_xll.RtGet(SourceAlias,$L26,Q$2)-Q26),0)</f>
-        <v>9.9999999999749734E-3</v>
+        <v>1.1823875212257917E-14</v>
       </c>
       <c r="U26" s="54">
         <f>IF($K26,ABS(_xll.RtGet(SourceAlias,$L26,R$2)-R26),0)</f>
-        <v>9.9999999999749734E-3</v>
+        <v>1.1823875212257917E-14</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4301,23 +4306,23 @@
       <c r="M27" s="55"/>
       <c r="N27" s="55">
         <f>_xll.qlInterestRateIndexFixingDate(H27,O27)</f>
-        <v>41919</v>
+        <v>42101</v>
       </c>
       <c r="O27" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,$O$21,A27,,TRUE)</f>
-        <v>41919</v>
+        <v>42101</v>
       </c>
       <c r="P27" s="55">
         <f>_xll.qlInterestRateIndexMaturity(H27,O27)</f>
-        <v>42011</v>
+        <v>42192</v>
       </c>
       <c r="Q27" s="56">
         <f>_xll.qlIndexFixing(H27,N27,,TriggerCounter)*100</f>
-        <v>0.45999999999995073</v>
+        <v>0.46084848214869978</v>
       </c>
       <c r="R27" s="56">
         <f t="shared" si="1"/>
-        <v>0.45999999999995073</v>
+        <v>0.46084848214869978</v>
       </c>
       <c r="S27" s="57" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K27),_xll.RtContribute(SourceAlias,$L27,Fields,Q27:R27,"SCOPE:SERVER"),"--")</f>
@@ -4325,11 +4330,11 @@
       </c>
       <c r="T27" s="56">
         <f>IF($K27,ABS(_xll.RtGet(SourceAlias,$L27,Q$2)-Q27),0)</f>
-        <v>1.0000000000049247E-2</v>
+        <v>8.4848214869975846E-4</v>
       </c>
       <c r="U27" s="58">
         <f>IF($K27,ABS(_xll.RtGet(SourceAlias,$L27,R$2)-R27),0)</f>
-        <v>1.0000000000049247E-2</v>
+        <v>8.4848214869975846E-4</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4368,27 +4373,27 @@
       </c>
       <c r="M28" s="47" t="str">
         <f>_xll.qlSwapIndex(,,B28,J28,Currency,Calendar,E28,"mf",F28,H28,$F$19,,Trigger)</f>
-        <v>obj_00182#0000</v>
+        <v>obj_0019f#0000</v>
       </c>
       <c r="N28" s="47">
         <f>EvaluationDate</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O28" s="47">
         <f>_xll.qlInterestRateIndexValueDate(M28,N28)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="P28" s="47">
         <f>_xll.qlInterestRateIndexMaturity(M28,O28)</f>
-        <v>42102</v>
+        <v>42284</v>
       </c>
       <c r="Q28" s="63">
         <f>_xll.qlIndexFixing(M28,N28,,TriggerCounter)*100</f>
-        <v>0.44510365513847161</v>
+        <v>0.47700583105270639</v>
       </c>
       <c r="R28" s="48">
         <f t="shared" si="1"/>
-        <v>0.44510365513847161</v>
+        <v>0.47700583105270639</v>
       </c>
       <c r="S28" s="49" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K28),_xll.RtContribute(SourceAlias,$L28,Fields,Q28:R28,"SCOPE:SERVER"),"--")</f>
@@ -4396,11 +4401,11 @@
       </c>
       <c r="T28" s="48">
         <f>IF($K28,ABS(_xll.RtGet(SourceAlias,$L28,Q$2)-Q28),0)</f>
-        <v>8.9834278615283925E-3</v>
+        <v>4.6570570527063593E-3</v>
       </c>
       <c r="U28" s="50">
         <f>IF($K28,ABS(_xll.RtGet(SourceAlias,$L28,R$2)-R28),0)</f>
-        <v>8.9834278615283925E-3</v>
+        <v>4.6570570527063593E-3</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4439,27 +4444,27 @@
       </c>
       <c r="M29" s="51" t="str">
         <f>_xll.qlSwapIndex(,,B29,J29,Currency,Calendar,E29,"mf",F29,H29,$F$19,,Trigger)</f>
-        <v>obj_0019c#0000</v>
+        <v>obj_001b6#0000</v>
       </c>
       <c r="N29" s="51">
         <f t="shared" ref="N29:N37" si="2">EvaluationDate</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O29" s="51">
         <f>_xll.qlInterestRateIndexValueDate(M29,N29)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="P29" s="51">
         <f>_xll.qlInterestRateIndexMaturity(M29,O29)</f>
-        <v>42285</v>
+        <v>42467</v>
       </c>
       <c r="Q29" s="52">
         <f>_xll.qlIndexFixing(M29,N29,,TriggerCounter)*100</f>
-        <v>0.54378034574071332</v>
+        <v>0.68175478973741643</v>
       </c>
       <c r="R29" s="52">
         <f t="shared" si="1"/>
-        <v>0.54378034574071332</v>
+        <v>0.68175478973741643</v>
       </c>
       <c r="S29" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K29),_xll.RtContribute(SourceAlias,$L29,Fields,Q29:R29,"SCOPE:SERVER"),"--")</f>
@@ -4467,11 +4472,11 @@
       </c>
       <c r="T29" s="52">
         <f>IF($K29,ABS(_xll.RtGet(SourceAlias,$L29,Q$2)-Q29),0)</f>
-        <v>3.2101290259286652E-2</v>
+        <v>9.2740577374164079E-3</v>
       </c>
       <c r="U29" s="54">
         <f>IF($K29,ABS(_xll.RtGet(SourceAlias,$L29,R$2)-R29),0)</f>
-        <v>3.2101290259286652E-2</v>
+        <v>9.2740577374164079E-3</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4510,27 +4515,27 @@
       </c>
       <c r="M30" s="51" t="str">
         <f>_xll.qlSwapIndex(,,B30,J30,Currency,Calendar,E30,"mf",F30,H30,$F$19,,Trigger)</f>
-        <v>obj_00184#0000</v>
+        <v>obj_001a9#0000</v>
       </c>
       <c r="N30" s="51">
         <f t="shared" si="2"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O30" s="51">
         <f>_xll.qlInterestRateIndexValueDate(M30,N30)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="P30" s="51">
         <f>_xll.qlInterestRateIndexMaturity(M30,O30)</f>
-        <v>42468</v>
+        <v>42650</v>
       </c>
       <c r="Q30" s="52">
         <f>_xll.qlIndexFixing(M30,N30,,TriggerCounter)*100</f>
-        <v>0.71612232308778634</v>
+        <v>0.89194603309716791</v>
       </c>
       <c r="R30" s="52">
         <f t="shared" si="1"/>
-        <v>0.71612232308778634</v>
+        <v>0.89194603309716791</v>
       </c>
       <c r="S30" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K30),_xll.RtContribute(SourceAlias,$L30,Fields,Q30:R30,"SCOPE:SERVER"),"--")</f>
@@ -4538,11 +4543,11 @@
       </c>
       <c r="T30" s="52">
         <f>IF($K30,ABS(_xll.RtGet(SourceAlias,$L30,Q$2)-Q30),0)</f>
-        <v>3.9622359912213634E-2</v>
+        <v>6.749374097167915E-3</v>
       </c>
       <c r="U30" s="54">
         <f>IF($K30,ABS(_xll.RtGet(SourceAlias,$L30,R$2)-R30),0)</f>
-        <v>3.9622359912213634E-2</v>
+        <v>6.749374097167915E-3</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4581,27 +4586,27 @@
       </c>
       <c r="M31" s="51" t="str">
         <f>_xll.qlSwapIndex(,,B31,J31,Currency,Calendar,E31,"mf",F31,H31,$F$19,,Trigger)</f>
-        <v>obj_00195#0000</v>
+        <v>obj_001a6#0000</v>
       </c>
       <c r="N31" s="51">
         <f t="shared" si="2"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O31" s="51">
         <f>_xll.qlInterestRateIndexValueDate(M31,N31)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="P31" s="51">
         <f>_xll.qlInterestRateIndexMaturity(M31,O31)</f>
-        <v>42835</v>
+        <v>43017</v>
       </c>
       <c r="Q31" s="52">
         <f>_xll.qlIndexFixing(M31,N31,,TriggerCounter)*100</f>
-        <v>1.1684865164871101</v>
+        <v>1.354190871447118</v>
       </c>
       <c r="R31" s="52">
         <f t="shared" si="1"/>
-        <v>1.1684865164871101</v>
+        <v>1.354190871447118</v>
       </c>
       <c r="S31" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K31),_xll.RtContribute(SourceAlias,$L31,Fields,Q31:R31,"SCOPE:SERVER"),"--")</f>
@@ -4609,11 +4614,11 @@
       </c>
       <c r="T31" s="52">
         <f>IF($K31,ABS(_xll.RtGet(SourceAlias,$L31,Q$2)-Q31),0)</f>
-        <v>3.9954269512889828E-2</v>
+        <v>5.9918684471180761E-3</v>
       </c>
       <c r="U31" s="54">
         <f>IF($K31,ABS(_xll.RtGet(SourceAlias,$L31,R$2)-R31),0)</f>
-        <v>3.9954269512889828E-2</v>
+        <v>5.9918684471180761E-3</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4652,27 +4657,27 @@
       </c>
       <c r="M32" s="51" t="str">
         <f>_xll.qlSwapIndex(,,B32,J32,Currency,Calendar,E32,"mf",F32,H32,$F$19,,Trigger)</f>
-        <v>obj_0019e#0000</v>
+        <v>obj_001b1#0000</v>
       </c>
       <c r="N32" s="51">
         <f t="shared" si="2"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O32" s="51">
         <f>_xll.qlInterestRateIndexValueDate(M32,N32)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="P32" s="51">
         <f>_xll.qlInterestRateIndexMaturity(M32,O32)</f>
-        <v>43199</v>
+        <v>43381</v>
       </c>
       <c r="Q32" s="52">
         <f>_xll.qlIndexFixing(M32,N32,,TriggerCounter)*100</f>
-        <v>1.5673006347734588</v>
+        <v>1.6709071477808817</v>
       </c>
       <c r="R32" s="52">
         <f t="shared" si="1"/>
-        <v>1.5673006347734588</v>
+        <v>1.6709071477808817</v>
       </c>
       <c r="S32" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K32),_xll.RtContribute(SourceAlias,$L32,Fields,Q32:R32,"SCOPE:SERVER"),"--")</f>
@@ -4680,11 +4685,11 @@
       </c>
       <c r="T32" s="52">
         <f>IF($K32,ABS(_xll.RtGet(SourceAlias,$L32,Q$2)-Q32),0)</f>
-        <v>6.093232022654127E-2</v>
+        <v>3.4293057808816307E-3</v>
       </c>
       <c r="U32" s="54">
         <f>IF($K32,ABS(_xll.RtGet(SourceAlias,$L32,R$2)-R32),0)</f>
-        <v>6.093232022654127E-2</v>
+        <v>3.4293057808816307E-3</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4723,27 +4728,27 @@
       </c>
       <c r="M33" s="51" t="str">
         <f>_xll.qlSwapIndex(,,B33,J33,Currency,Calendar,E33,"mf",F33,H33,$F$19,,Trigger)</f>
-        <v>obj_0018a#0000</v>
+        <v>obj_001ba#0000</v>
       </c>
       <c r="N33" s="51">
         <f t="shared" si="2"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O33" s="51">
         <f>_xll.qlInterestRateIndexValueDate(M33,N33)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="P33" s="51">
         <f>_xll.qlInterestRateIndexMaturity(M33,O33)</f>
-        <v>43563</v>
+        <v>43745</v>
       </c>
       <c r="Q33" s="52">
         <f>_xll.qlIndexFixing(M33,N33,,TriggerCounter)*100</f>
-        <v>1.8966236084002004</v>
+        <v>1.8908592292454673</v>
       </c>
       <c r="R33" s="52">
         <f t="shared" si="1"/>
-        <v>1.8966236084002004</v>
+        <v>1.8908592292454673</v>
       </c>
       <c r="S33" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K33),_xll.RtContribute(SourceAlias,$L33,Fields,Q33:R33,"SCOPE:SERVER"),"--")</f>
@@ -4751,11 +4756,11 @@
       </c>
       <c r="T33" s="52">
         <f>IF($K33,ABS(_xll.RtGet(SourceAlias,$L33,Q$2)-Q33),0)</f>
-        <v>5.9972222599799618E-2</v>
+        <v>3.6079152454673302E-3</v>
       </c>
       <c r="U33" s="54">
         <f>IF($K33,ABS(_xll.RtGet(SourceAlias,$L33,R$2)-R33),0)</f>
-        <v>5.9972222599799618E-2</v>
+        <v>3.6079152454673302E-3</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4794,27 +4799,27 @@
       </c>
       <c r="M34" s="51" t="str">
         <f>_xll.qlSwapIndex(,,B34,J34,Currency,Calendar,E34,"mf",F34,H34,$F$19,,Trigger)</f>
-        <v>obj_0018c#0000</v>
+        <v>obj_001ab#0000</v>
       </c>
       <c r="N34" s="51">
         <f t="shared" si="2"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O34" s="51">
         <f>_xll.qlInterestRateIndexValueDate(M34,N34)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="P34" s="51">
         <f>_xll.qlInterestRateIndexMaturity(M34,O34)</f>
-        <v>44294</v>
+        <v>44476</v>
       </c>
       <c r="Q34" s="52">
         <f>_xll.qlIndexFixing(M34,N34,,TriggerCounter)*100</f>
-        <v>2.3662940927485843</v>
+        <v>2.1810631536777212</v>
       </c>
       <c r="R34" s="52">
         <f t="shared" si="1"/>
-        <v>2.3662940927485843</v>
+        <v>2.1810631536777212</v>
       </c>
       <c r="S34" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K34),_xll.RtContribute(SourceAlias,$L34,Fields,Q34:R34,"SCOPE:SERVER"),"--")</f>
@@ -4822,11 +4827,11 @@
       </c>
       <c r="T34" s="52">
         <f>IF($K34,ABS(_xll.RtGet(SourceAlias,$L34,Q$2)-Q34),0)</f>
-        <v>4.9575952251415867E-2</v>
+        <v>3.8144146777212562E-3</v>
       </c>
       <c r="U34" s="54">
         <f>IF($K34,ABS(_xll.RtGet(SourceAlias,$L34,R$2)-R34),0)</f>
-        <v>4.9575952251415867E-2</v>
+        <v>3.8144146777212562E-3</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4865,27 +4870,27 @@
       </c>
       <c r="M35" s="51" t="str">
         <f>_xll.qlSwapIndex(,,B35,J35,Currency,Calendar,E35,"mf",F35,H35,$F$19,,Trigger)</f>
-        <v>obj_00188#0000</v>
+        <v>obj_001bb#0000</v>
       </c>
       <c r="N35" s="51">
         <f t="shared" si="2"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O35" s="51">
         <f>_xll.qlInterestRateIndexValueDate(M35,N35)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="P35" s="51">
         <f>_xll.qlInterestRateIndexMaturity(M35,O35)</f>
-        <v>45390</v>
+        <v>45572</v>
       </c>
       <c r="Q35" s="52">
         <f>_xll.qlIndexFixing(M35,N35,,TriggerCounter)*100</f>
-        <v>2.7779515654998677</v>
+        <v>2.4406257466169796</v>
       </c>
       <c r="R35" s="52">
         <f t="shared" si="1"/>
-        <v>2.7779515654998677</v>
+        <v>2.4406257466169796</v>
       </c>
       <c r="S35" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K35),_xll.RtContribute(SourceAlias,$L35,Fields,Q35:R35,"SCOPE:SERVER"),"--")</f>
@@ -4893,11 +4898,11 @@
       </c>
       <c r="T35" s="52">
         <f>IF($K35,ABS(_xll.RtGet(SourceAlias,$L35,Q$2)-Q35),0)</f>
-        <v>3.0271456500132299E-2</v>
+        <v>2.2399766169796109E-3</v>
       </c>
       <c r="U35" s="54">
         <f>IF($K35,ABS(_xll.RtGet(SourceAlias,$L35,R$2)-R35),0)</f>
-        <v>3.0271456500132299E-2</v>
+        <v>2.2399766169796109E-3</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4936,27 +4941,27 @@
       </c>
       <c r="M36" s="51" t="str">
         <f>_xll.qlSwapIndex(,,B36,J36,Currency,Calendar,E36,"mf",F36,H36,$F$19,,Trigger)</f>
-        <v>obj_00187#0000</v>
+        <v>obj_001b5#0000</v>
       </c>
       <c r="N36" s="51">
         <f t="shared" si="2"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O36" s="51">
         <f>_xll.qlInterestRateIndexValueDate(M36,N36)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="P36" s="51">
         <f>_xll.qlInterestRateIndexMaturity(M36,O36)</f>
-        <v>46120</v>
+        <v>46302</v>
       </c>
       <c r="Q36" s="52">
         <f>_xll.qlIndexFixing(M36,N36,,TriggerCounter)*100</f>
-        <v>2.9383391129345471</v>
+        <v>2.5506889398321815</v>
       </c>
       <c r="R36" s="52">
         <f t="shared" si="1"/>
-        <v>2.9383391129345471</v>
+        <v>2.5506889398321815</v>
       </c>
       <c r="S36" s="53" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K36),_xll.RtContribute(SourceAlias,$L36,Fields,Q36:R36,"SCOPE:SERVER"),"--")</f>
@@ -4964,11 +4969,11 @@
       </c>
       <c r="T36" s="52">
         <f>IF($K36,ABS(_xll.RtGet(SourceAlias,$L36,Q$2)-Q36),0)</f>
-        <v>3.9301865065453079E-2</v>
+        <v>2.0638488321815807E-3</v>
       </c>
       <c r="U36" s="54">
         <f>IF($K36,ABS(_xll.RtGet(SourceAlias,$L36,R$2)-R36),0)</f>
-        <v>3.9301865065453079E-2</v>
+        <v>2.0638488321815807E-3</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5007,27 +5012,27 @@
       </c>
       <c r="M37" s="55" t="str">
         <f>_xll.qlSwapIndex(,,B37,J37,Currency,Calendar,E37,"mf",F37,H37,$F$19,,Trigger)</f>
-        <v>obj_00198#0000</v>
+        <v>obj_001b8#0000</v>
       </c>
       <c r="N37" s="55">
         <f t="shared" si="2"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O37" s="55">
         <f>_xll.qlInterestRateIndexValueDate(M37,N37)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="P37" s="55">
         <f>_xll.qlInterestRateIndexMaturity(M37,O37)</f>
-        <v>47217</v>
+        <v>47399</v>
       </c>
       <c r="Q37" s="56">
         <f>_xll.qlIndexFixing(M37,N37,,TriggerCounter)*100</f>
-        <v>3.0187806493853597</v>
+        <v>2.6504930563202094</v>
       </c>
       <c r="R37" s="56">
         <f t="shared" si="1"/>
-        <v>3.0187806493853597</v>
+        <v>2.6504930563202094</v>
       </c>
       <c r="S37" s="57" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K37),_xll.RtContribute(SourceAlias,$L37,Fields,Q37:R37,"SCOPE:SERVER"),"--")</f>
@@ -5035,11 +5040,11 @@
       </c>
       <c r="T37" s="56">
         <f>IF($K37,ABS(_xll.RtGet(SourceAlias,$L37,Q$2)-Q37),0)</f>
-        <v>5.0022173614640231E-2</v>
+        <v>1.5489833202093628E-3</v>
       </c>
       <c r="U37" s="58">
         <f>IF($K37,ABS(_xll.RtGet(SourceAlias,$L37,R$2)-R37),0)</f>
-        <v>5.0022173614640231E-2</v>
+        <v>1.5489833202093628E-3</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5107,19 +5112,19 @@
       <c r="N39" s="5"/>
       <c r="O39" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J39)</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="P39" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O39,"1d",,TRUE)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="Q39" s="19">
         <f>(_xll.qlYieldTSDiscount($F$38,O39,TriggerCounter)/_xll.qlYieldTSDiscount($F$38,P39)-1)/_xll.qlDayCounterYearFraction(F39,O39,P39)*100</f>
-        <v>0.54782110762929825</v>
+        <v>0.66687071426552169</v>
       </c>
       <c r="R39" s="19">
         <f t="shared" si="1"/>
-        <v>0.54782110762929825</v>
+        <v>0.66687071426552169</v>
       </c>
       <c r="S39" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K39),_xll.RtContribute(SourceAlias,$L39,Fields,Q39:R39,"SCOPE:SERVER"),"--")</f>
@@ -5127,11 +5132,11 @@
       </c>
       <c r="T39" s="19">
         <f>IF($K39,ABS(_xll.RtGet(SourceAlias,$L39,Q$2)-Q39),0)</f>
-        <v>3.7070169156550037E-10</v>
+        <v>2.6552171572546968E-10</v>
       </c>
       <c r="U39" s="19">
         <f>IF($K39,ABS(_xll.RtGet(SourceAlias,$L39,R$2)-R39),0)</f>
-        <v>3.7070169156550037E-10</v>
+        <v>2.6552171572546968E-10</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5172,19 +5177,19 @@
       <c r="N40" s="5"/>
       <c r="O40" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J40)</f>
-        <v>41738</v>
+        <v>41920</v>
       </c>
       <c r="P40" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O40,B40,,TRUE)</f>
-        <v>41745</v>
+        <v>41927</v>
       </c>
       <c r="Q40" s="19">
         <f>(_xll.qlYieldTSDiscount($F$38,O40,TriggerCounter)/_xll.qlYieldTSDiscount($F$38,P40)-1)/_xll.qlDayCounterYearFraction(F40,O40,P40)*100</f>
-        <v>0.54784577465533901</v>
+        <v>0.66650554914057403</v>
       </c>
       <c r="R40" s="19">
         <f t="shared" si="1"/>
-        <v>0.54784577465533901</v>
+        <v>0.66650554914057403</v>
       </c>
       <c r="S40" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K40),_xll.RtContribute(SourceAlias,$L40,Fields,Q40:R40,"SCOPE:SERVER"),"--")</f>
@@ -5192,11 +5197,11 @@
       </c>
       <c r="T40" s="19">
         <f>IF($K40,ABS(_xll.RtGet(SourceAlias,$L40,Q$2)-Q40),0)</f>
-        <v>3.4466096643370747E-10</v>
+        <v>1.4057399688738315E-10</v>
       </c>
       <c r="U40" s="19">
         <f>IF($K40,ABS(_xll.RtGet(SourceAlias,$L40,R$2)-R40),0)</f>
-        <v>3.4466096643370747E-10</v>
+        <v>1.4057399688738315E-10</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5237,19 +5242,19 @@
       <c r="N41" s="5"/>
       <c r="O41" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J41)</f>
-        <v>41738</v>
+        <v>41920</v>
       </c>
       <c r="P41" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O41,B41,,TRUE)</f>
-        <v>41752</v>
+        <v>41934</v>
       </c>
       <c r="Q41" s="19">
         <f>(_xll.qlYieldTSDiscount($F$38,O41,TriggerCounter)/_xll.qlYieldTSDiscount($F$38,P41)-1)/_xll.qlDayCounterYearFraction(F41,O41,P41)*100</f>
-        <v>0.54787455472281898</v>
+        <v>0.66580369114091087</v>
       </c>
       <c r="R41" s="19">
         <f t="shared" si="1"/>
-        <v>0.54787455472281898</v>
+        <v>0.66580369114091087</v>
       </c>
       <c r="S41" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K41),_xll.RtContribute(SourceAlias,$L41,Fields,Q41:R41,"SCOPE:SERVER"),"--")</f>
@@ -5257,11 +5262,11 @@
       </c>
       <c r="T41" s="19">
         <f>IF($K41,ABS(_xll.RtGet(SourceAlias,$L41,Q$2)-Q41),0)</f>
-        <v>2.7718105588547814E-10</v>
+        <v>1.4091083855305442E-10</v>
       </c>
       <c r="U41" s="19">
         <f>IF($K41,ABS(_xll.RtGet(SourceAlias,$L41,R$2)-R41),0)</f>
-        <v>2.7718105588547814E-10</v>
+        <v>1.4091083855305442E-10</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5302,19 +5307,19 @@
       <c r="N42" s="5"/>
       <c r="O42" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J42)</f>
-        <v>41738</v>
+        <v>41920</v>
       </c>
       <c r="P42" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O42,B42,,TRUE)</f>
-        <v>41768</v>
+        <v>41953</v>
       </c>
       <c r="Q42" s="19">
         <f>(_xll.qlYieldTSDiscount($F$38,O42,TriggerCounter)/_xll.qlYieldTSDiscount($F$38,P42)-1)/_xll.qlDayCounterYearFraction(F42,O42,P42)*100</f>
-        <v>0.54794034530523117</v>
+        <v>0.66195121589481443</v>
       </c>
       <c r="R42" s="19">
         <f t="shared" si="1"/>
-        <v>0.54794034530523117</v>
+        <v>0.66195121589481443</v>
       </c>
       <c r="S42" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K42),_xll.RtContribute(SourceAlias,$L42,Fields,Q42:R42,"SCOPE:SERVER"),"--")</f>
@@ -5322,11 +5327,11 @@
       </c>
       <c r="T42" s="19">
         <f>IF($K42,ABS(_xll.RtGet(SourceAlias,$L42,Q$2)-Q42),0)</f>
-        <v>3.0523117366954011E-10</v>
+        <v>8.9481444476291472E-10</v>
       </c>
       <c r="U42" s="19">
         <f>IF($K42,ABS(_xll.RtGet(SourceAlias,$L42,R$2)-R42),0)</f>
-        <v>3.0523117366954011E-10</v>
+        <v>8.9481444476291472E-10</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5367,19 +5372,19 @@
       <c r="N43" s="5"/>
       <c r="O43" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J43)</f>
-        <v>41738</v>
+        <v>41920</v>
       </c>
       <c r="P43" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O43,B43,,TRUE)</f>
-        <v>41799</v>
+        <v>41981</v>
       </c>
       <c r="Q43" s="19">
         <f>(_xll.qlYieldTSDiscount($F$38,O43,TriggerCounter)/_xll.qlYieldTSDiscount($F$38,P43)-1)/_xll.qlDayCounterYearFraction(F43,O43,P43)*100</f>
-        <v>0.54806784453620783</v>
+        <v>0.65108102933429413</v>
       </c>
       <c r="R43" s="19">
         <f t="shared" si="1"/>
-        <v>0.54806784453620783</v>
+        <v>0.65108102933429413</v>
       </c>
       <c r="S43" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K43),_xll.RtContribute(SourceAlias,$L43,Fields,Q43:R43,"SCOPE:SERVER"),"--")</f>
@@ -5387,11 +5392,11 @@
       </c>
       <c r="T43" s="19">
         <f>IF($K43,ABS(_xll.RtGet(SourceAlias,$L43,Q$2)-Q43),0)</f>
-        <v>4.1134637921436124E-6</v>
+        <v>3.3429414791896761E-10</v>
       </c>
       <c r="U43" s="19">
         <f>IF($K43,ABS(_xll.RtGet(SourceAlias,$L43,R$2)-R43),0)</f>
-        <v>4.1134637921436124E-6</v>
+        <v>3.3429414791896761E-10</v>
       </c>
     </row>
     <row r="44" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5432,19 +5437,19 @@
       <c r="N44" s="5"/>
       <c r="O44" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J44)</f>
-        <v>41738</v>
+        <v>41920</v>
       </c>
       <c r="P44" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O44,B44,,TRUE)</f>
-        <v>41829</v>
+        <v>42012</v>
       </c>
       <c r="Q44" s="19">
         <f>(_xll.qlYieldTSDiscount($F$38,O44,TriggerCounter)/_xll.qlYieldTSDiscount($F$38,P44)-1)/_xll.qlDayCounterYearFraction(F44,O44,P44)*100</f>
-        <v>0.5481912685518201</v>
+        <v>0.63181966219099728</v>
       </c>
       <c r="R44" s="19">
         <f t="shared" si="1"/>
-        <v>0.5481912685518201</v>
+        <v>0.63181966219099728</v>
       </c>
       <c r="S44" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K44),_xll.RtContribute(SourceAlias,$L44,Fields,Q44:R44,"SCOPE:SERVER"),"--")</f>
@@ -5452,11 +5457,11 @@
       </c>
       <c r="T44" s="19">
         <f>IF($K44,ABS(_xll.RtGet(SourceAlias,$L44,Q$2)-Q44),0)</f>
-        <v>4.4817993760659647E-10</v>
+        <v>1.9099732906369127E-10</v>
       </c>
       <c r="U44" s="19">
         <f>IF($K44,ABS(_xll.RtGet(SourceAlias,$L44,R$2)-R44),0)</f>
-        <v>4.4817993760659647E-10</v>
+        <v>1.9099732906369127E-10</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5497,19 +5502,19 @@
       <c r="N45" s="5"/>
       <c r="O45" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J45)</f>
-        <v>41738</v>
+        <v>41920</v>
       </c>
       <c r="P45" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O45,B45,,TRUE)</f>
-        <v>41862</v>
+        <v>42044</v>
       </c>
       <c r="Q45" s="19">
         <f>(_xll.qlYieldTSDiscount($F$38,O45,TriggerCounter)/_xll.qlYieldTSDiscount($F$38,P45)-1)/_xll.qlDayCounterYearFraction(F45,O45,P45)*100</f>
-        <v>0.54832707777194023</v>
+        <v>0.60396094018236224</v>
       </c>
       <c r="R45" s="19">
         <f t="shared" si="1"/>
-        <v>0.54832707777194023</v>
+        <v>0.60396094018236224</v>
       </c>
       <c r="S45" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K45),_xll.RtContribute(SourceAlias,$L45,Fields,Q45:R45,"SCOPE:SERVER"),"--")</f>
@@ -5517,11 +5522,11 @@
       </c>
       <c r="T45" s="19">
         <f>IF($K45,ABS(_xll.RtGet(SourceAlias,$L45,Q$2)-Q45),0)</f>
-        <v>2.2805979327245041E-10</v>
+        <v>1.8236223642276173E-10</v>
       </c>
       <c r="U45" s="19">
         <f>IF($K45,ABS(_xll.RtGet(SourceAlias,$L45,R$2)-R45),0)</f>
-        <v>2.2805979327245041E-10</v>
+        <v>1.8236223642276173E-10</v>
       </c>
     </row>
     <row r="46" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5562,19 +5567,19 @@
       <c r="N46" s="5"/>
       <c r="O46" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J46)</f>
-        <v>41738</v>
+        <v>41920</v>
       </c>
       <c r="P46" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O46,B46,,TRUE)</f>
-        <v>41892</v>
+        <v>42072</v>
       </c>
       <c r="Q46" s="19">
         <f>(_xll.qlYieldTSDiscount($F$38,O46,TriggerCounter)/_xll.qlYieldTSDiscount($F$38,P46)-1)/_xll.qlDayCounterYearFraction(F46,O46,P46)*100</f>
-        <v>0.54845057962470301</v>
+        <v>0.57293082712937959</v>
       </c>
       <c r="R46" s="19">
         <f t="shared" si="1"/>
-        <v>0.54845057962470301</v>
+        <v>0.57293082712937959</v>
       </c>
       <c r="S46" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K46),_xll.RtContribute(SourceAlias,$L46,Fields,Q46:R46,"SCOPE:SERVER"),"--")</f>
@@ -5582,11 +5587,11 @@
       </c>
       <c r="T46" s="19">
         <f>IF($K46,ABS(_xll.RtGet(SourceAlias,$L46,Q$2)-Q46),0)</f>
-        <v>4.1176247029817148E-6</v>
+        <v>1.2937961813008769E-10</v>
       </c>
       <c r="U46" s="19">
         <f>IF($K46,ABS(_xll.RtGet(SourceAlias,$L46,R$2)-R46),0)</f>
-        <v>4.1176247029817148E-6</v>
+        <v>1.2937961813008769E-10</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5627,19 +5632,19 @@
       <c r="N47" s="5"/>
       <c r="O47" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J47)</f>
-        <v>41738</v>
+        <v>41920</v>
       </c>
       <c r="P47" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O47,B47,,TRUE)</f>
-        <v>41921</v>
+        <v>42102</v>
       </c>
       <c r="Q47" s="19">
         <f>(_xll.qlYieldTSDiscount($F$38,O47,TriggerCounter)/_xll.qlYieldTSDiscount($F$38,P47)-1)/_xll.qlDayCounterYearFraction(F47,O47,P47)*100</f>
-        <v>0.54412103704445369</v>
+        <v>0.53278898908975225</v>
       </c>
       <c r="R47" s="19">
         <f t="shared" si="1"/>
-        <v>0.54412103704445369</v>
+        <v>0.53278898908975225</v>
       </c>
       <c r="S47" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K47),_xll.RtContribute(SourceAlias,$L47,Fields,Q47:R47,"SCOPE:SERVER"),"--")</f>
@@ -5647,11 +5652,11 @@
       </c>
       <c r="T47" s="19">
         <f>IF($K47,ABS(_xll.RtGet(SourceAlias,$L47,Q$2)-Q47),0)</f>
-        <v>1.2161350444537256E-3</v>
+        <v>8.9752205667537055E-11</v>
       </c>
       <c r="U47" s="19">
         <f>IF($K47,ABS(_xll.RtGet(SourceAlias,$L47,R$2)-R47),0)</f>
-        <v>1.2161350444537256E-3</v>
+        <v>8.9752205667537055E-11</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5694,23 +5699,23 @@
       <c r="M48" s="5"/>
       <c r="N48" s="5">
         <f>_xll.qlInterestRateIndexFixingDate(H48,O48)</f>
-        <v>41768</v>
+        <v>41953</v>
       </c>
       <c r="O48" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,$O$40,A48,,TRUE)</f>
-        <v>41768</v>
+        <v>41953</v>
       </c>
       <c r="P48" s="5">
         <f>_xll.qlInterestRateIndexMaturity(H48,O48)</f>
-        <v>41953</v>
+        <v>42135</v>
       </c>
       <c r="Q48" s="19">
         <f>_xll.qlIndexFixing(H48,N48,,TriggerCounter)*100</f>
-        <v>0.48226350141848229</v>
+        <v>0.47788269244646125</v>
       </c>
       <c r="R48" s="19">
         <f t="shared" si="1"/>
-        <v>0.48226350141848229</v>
+        <v>0.47788269244646125</v>
       </c>
       <c r="S48" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K48),_xll.RtContribute(SourceAlias,$L48,Fields,Q48:R48,"SCOPE:SERVER"),"--")</f>
@@ -5718,11 +5723,11 @@
       </c>
       <c r="T48" s="19">
         <f>IF($K48,ABS(_xll.RtGet(SourceAlias,$L48,Q$2)-Q48),0)</f>
-        <v>7.0707685815177279E-3</v>
+        <v>5.5353877037589427E-10</v>
       </c>
       <c r="U48" s="19">
         <f>IF($K48,ABS(_xll.RtGet(SourceAlias,$L48,R$2)-R48),0)</f>
-        <v>7.0707685815177279E-3</v>
+        <v>5.5353877037589427E-10</v>
       </c>
     </row>
     <row r="49" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5765,23 +5770,23 @@
       <c r="M49" s="5"/>
       <c r="N49" s="5">
         <f>_xll.qlInterestRateIndexFixingDate(H49,O49)</f>
-        <v>41799</v>
+        <v>41981</v>
       </c>
       <c r="O49" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,$O$40,A49,,TRUE)</f>
-        <v>41799</v>
+        <v>41981</v>
       </c>
       <c r="P49" s="5">
         <f>_xll.qlInterestRateIndexMaturity(H49,O49)</f>
-        <v>41982</v>
+        <v>42163</v>
       </c>
       <c r="Q49" s="19">
         <f>_xll.qlIndexFixing(H49,N49,,TriggerCounter)*100</f>
-        <v>0.4999999999995815</v>
+        <v>0.4899999999861816</v>
       </c>
       <c r="R49" s="19">
         <f t="shared" si="1"/>
-        <v>0.4999999999995815</v>
+        <v>0.4899999999861816</v>
       </c>
       <c r="S49" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K49),_xll.RtContribute(SourceAlias,$L49,Fields,Q49:R49,"SCOPE:SERVER"),"--")</f>
@@ -5789,11 +5794,11 @@
       </c>
       <c r="T49" s="19">
         <f>IF($K49,ABS(_xll.RtGet(SourceAlias,$L49,Q$2)-Q49),0)</f>
-        <v>1.3643576999581519E-2</v>
+        <v>1.3818390875997011E-11</v>
       </c>
       <c r="U49" s="19">
         <f>IF($K49,ABS(_xll.RtGet(SourceAlias,$L49,R$2)-R49),0)</f>
-        <v>1.3643576999581519E-2</v>
+        <v>1.3818390875997011E-11</v>
       </c>
     </row>
     <row r="50" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5836,23 +5841,23 @@
       <c r="M50" s="5"/>
       <c r="N50" s="5">
         <f>_xll.qlInterestRateIndexFixingDate(H50,O50)</f>
-        <v>41829</v>
+        <v>42012</v>
       </c>
       <c r="O50" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,$O$40,A50,,TRUE)</f>
-        <v>41829</v>
+        <v>42012</v>
       </c>
       <c r="P50" s="5">
         <f>_xll.qlInterestRateIndexMaturity(H50,O50)</f>
-        <v>42013</v>
+        <v>42193</v>
       </c>
       <c r="Q50" s="19">
         <f>_xll.qlIndexFixing(H50,N50,,TriggerCounter)*100</f>
-        <v>0.51119935876036759</v>
+        <v>0.51197531004946761</v>
       </c>
       <c r="R50" s="19">
         <f t="shared" si="1"/>
-        <v>0.51119935876036759</v>
+        <v>0.51197531004946761</v>
       </c>
       <c r="S50" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K50),_xll.RtContribute(SourceAlias,$L50,Fields,Q50:R50,"SCOPE:SERVER"),"--")</f>
@@ -5860,11 +5865,11 @@
       </c>
       <c r="T50" s="19">
         <f>IF($K50,ABS(_xll.RtGet(SourceAlias,$L50,Q$2)-Q50),0)</f>
-        <v>1.0137283239632366E-2</v>
+        <v>4.9467652196710787E-11</v>
       </c>
       <c r="U50" s="19">
         <f>IF($K50,ABS(_xll.RtGet(SourceAlias,$L50,R$2)-R50),0)</f>
-        <v>1.0137283239632366E-2</v>
+        <v>4.9467652196710787E-11</v>
       </c>
     </row>
     <row r="51" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5907,23 +5912,23 @@
       <c r="M51" s="5"/>
       <c r="N51" s="5">
         <f>_xll.qlInterestRateIndexFixingDate(H51,O51)</f>
-        <v>41862</v>
+        <v>42044</v>
       </c>
       <c r="O51" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,$O$40,A51,,TRUE)</f>
-        <v>41862</v>
+        <v>42044</v>
       </c>
       <c r="P51" s="5">
         <f>_xll.qlInterestRateIndexMaturity(H51,O51)</f>
-        <v>42046</v>
+        <v>42226</v>
       </c>
       <c r="Q51" s="19">
         <f>_xll.qlIndexFixing(H51,N51,,TriggerCounter)*100</f>
-        <v>0.5312333012078454</v>
+        <v>0.55549872135657929</v>
       </c>
       <c r="R51" s="19">
         <f t="shared" si="1"/>
-        <v>0.5312333012078454</v>
+        <v>0.55549872135657929</v>
       </c>
       <c r="S51" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K51),_xll.RtContribute(SourceAlias,$L51,Fields,Q51:R51,"SCOPE:SERVER"),"--")</f>
@@ -5931,11 +5936,11 @@
       </c>
       <c r="T51" s="19">
         <f>IF($K51,ABS(_xll.RtGet(SourceAlias,$L51,Q$2)-Q51),0)</f>
-        <v>1.2358856792154649E-2</v>
+        <v>3.5657932162536099E-10</v>
       </c>
       <c r="U51" s="19">
         <f>IF($K51,ABS(_xll.RtGet(SourceAlias,$L51,R$2)-R51),0)</f>
-        <v>1.2358856792154649E-2</v>
+        <v>3.5657932162536099E-10</v>
       </c>
     </row>
     <row r="52" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5978,23 +5983,23 @@
       <c r="M52" s="5"/>
       <c r="N52" s="5">
         <f>_xll.qlInterestRateIndexFixingDate(H52,O52)</f>
-        <v>41892</v>
+        <v>42072</v>
       </c>
       <c r="O52" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,$O$40,A52,,TRUE)</f>
-        <v>41892</v>
+        <v>42072</v>
       </c>
       <c r="P52" s="5">
         <f>_xll.qlInterestRateIndexMaturity(H52,O52)</f>
-        <v>42073</v>
+        <v>42256</v>
       </c>
       <c r="Q52" s="19">
         <f>_xll.qlIndexFixing(H52,N52,,TriggerCounter)*100</f>
-        <v>0.55104389080056548</v>
+        <v>0.59318432266464105</v>
       </c>
       <c r="R52" s="19">
         <f t="shared" si="1"/>
-        <v>0.55104389080056548</v>
+        <v>0.59318432266464105</v>
       </c>
       <c r="S52" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K52),_xll.RtContribute(SourceAlias,$L52,Fields,Q52:R52,"SCOPE:SERVER"),"--")</f>
@@ -6002,11 +6007,11 @@
       </c>
       <c r="T52" s="19">
         <f>IF($K52,ABS(_xll.RtGet(SourceAlias,$L52,Q$2)-Q52),0)</f>
-        <v>1.0900236199434477E-2</v>
+        <v>3.353589628218856E-10</v>
       </c>
       <c r="U52" s="19">
         <f>IF($K52,ABS(_xll.RtGet(SourceAlias,$L52,R$2)-R52),0)</f>
-        <v>1.0900236199434477E-2</v>
+        <v>3.353589628218856E-10</v>
       </c>
     </row>
     <row r="53" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6049,23 +6054,23 @@
       <c r="M53" s="5"/>
       <c r="N53" s="5">
         <f>_xll.qlInterestRateIndexFixingDate(H53,O53)</f>
-        <v>41921</v>
+        <v>42102</v>
       </c>
       <c r="O53" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,$O$40,A53,,TRUE)</f>
-        <v>41921</v>
+        <v>42102</v>
       </c>
       <c r="P53" s="5">
         <f>_xll.qlInterestRateIndexMaturity(H53,O53)</f>
-        <v>42103</v>
+        <v>42285</v>
       </c>
       <c r="Q53" s="19">
         <f>_xll.qlIndexFixing(H53,N53,,TriggerCounter)*100</f>
-        <v>0.58811384106303422</v>
+        <v>0.63192839196566641</v>
       </c>
       <c r="R53" s="19">
         <f t="shared" si="1"/>
-        <v>0.58811384106303422</v>
+        <v>0.63192839196566641</v>
       </c>
       <c r="S53" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K53),_xll.RtContribute(SourceAlias,$L53,Fields,Q53:R53,"SCOPE:SERVER"),"--")</f>
@@ -6073,11 +6078,11 @@
       </c>
       <c r="T53" s="19">
         <f>IF($K53,ABS(_xll.RtGet(SourceAlias,$L53,Q$2)-Q53),0)</f>
-        <v>1.1558712936965754E-2</v>
+        <v>3.4333536014230503E-11</v>
       </c>
       <c r="U53" s="19">
         <f>IF($K53,ABS(_xll.RtGet(SourceAlias,$L53,R$2)-R53),0)</f>
-        <v>1.1558712936965754E-2</v>
+        <v>3.4333536014230503E-11</v>
       </c>
     </row>
     <row r="54" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6120,23 +6125,23 @@
       <c r="M54" s="5"/>
       <c r="N54" s="5">
         <f>_xll.qlInterestRateIndexFixingDate(H54,O54)</f>
-        <v>42103</v>
+        <v>42285</v>
       </c>
       <c r="O54" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,$O$40,A54,,TRUE)</f>
-        <v>42103</v>
+        <v>42285</v>
       </c>
       <c r="P54" s="5">
         <f>_xll.qlInterestRateIndexMaturity(H54,O54)</f>
-        <v>42286</v>
+        <v>42468</v>
       </c>
       <c r="Q54" s="19">
         <f>_xll.qlIndexFixing(H54,N54,,TriggerCounter)*100</f>
-        <v>0.88404002696511708</v>
+        <v>1.210061871097559</v>
       </c>
       <c r="R54" s="19">
         <f t="shared" si="1"/>
-        <v>0.88404002696511708</v>
+        <v>1.210061871097559</v>
       </c>
       <c r="S54" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K54),_xll.RtContribute(SourceAlias,$L54,Fields,Q54:R54,"SCOPE:SERVER"),"--")</f>
@@ -6144,11 +6149,11 @@
       </c>
       <c r="T54" s="19">
         <f>IF($K54,ABS(_xll.RtGet(SourceAlias,$L54,Q$2)-Q54),0)</f>
-        <v>6.0327248034882874E-2</v>
+        <v>9.7559071932096231E-11</v>
       </c>
       <c r="U54" s="19">
         <f>IF($K54,ABS(_xll.RtGet(SourceAlias,$L54,R$2)-R54),0)</f>
-        <v>6.0327248034882874E-2</v>
+        <v>9.7559071932096231E-11</v>
       </c>
     </row>
     <row r="55" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6191,35 +6196,35 @@
       <c r="M55" s="5"/>
       <c r="N55" s="5">
         <f>_xll.qlInterestRateIndexFixingDate(H55,O55)</f>
-        <v>42286</v>
+        <v>42468</v>
       </c>
       <c r="O55" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,$O$40,A55,,TRUE)</f>
-        <v>42286</v>
+        <v>42468</v>
       </c>
       <c r="P55" s="5">
         <f>_xll.qlInterestRateIndexMaturity(H55,O55)</f>
-        <v>42471</v>
-      </c>
-      <c r="Q55" s="19" t="e">
+        <v>42653</v>
+      </c>
+      <c r="Q55" s="19">
         <f>_xll.qlIndexFixing(H55,N55,,TriggerCounter)*100</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R55" s="19" t="e">
+        <v>1.5912141784738734</v>
+      </c>
+      <c r="R55" s="19">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>1.5912141784738734</v>
       </c>
       <c r="S55" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K55),_xll.RtContribute(SourceAlias,$L55,Fields,Q55:R55,"SCOPE:SERVER"),"--")</f>
         <v>--</v>
       </c>
-      <c r="T55" s="19" t="e">
+      <c r="T55" s="19">
         <f>IF($K55,ABS(_xll.RtGet(SourceAlias,$L55,Q$2)-Q55),0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="U55" s="19" t="e">
+        <v>4.121417847387332E-2</v>
+      </c>
+      <c r="U55" s="19">
         <f>IF($K55,ABS(_xll.RtGet(SourceAlias,$L55,R$2)-R55),0)</f>
-        <v>#NUM!</v>
+        <v>4.121417847387332E-2</v>
       </c>
     </row>
     <row r="56" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6259,31 +6264,31 @@
       <c r="M56" s="5"/>
       <c r="N56" s="5">
         <f t="shared" ref="N56:N62" si="3">EvaluationDate</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O56" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B56,J56,Currency,Calendar,E56,"mf",F56,H56,$F$38,,Trigger)</f>
-        <v>obj_00199#0000</v>
-      </c>
-      <c r="Q56" s="19" t="e">
+        <v>obj_001b9#0000</v>
+      </c>
+      <c r="Q56" s="19">
         <f>_xll.qlIndexFixing(O56,N56,,TriggerCounter)*100</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R56" s="19" t="e">
+        <v>1.1950682191499502</v>
+      </c>
+      <c r="R56" s="19">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>1.1950682191499502</v>
       </c>
       <c r="S56" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K56),_xll.RtContribute(SourceAlias,$L56,Fields,Q56:R56,"SCOPE:SERVER"),"--")</f>
         <v>--</v>
       </c>
-      <c r="T56" s="19" t="e">
+      <c r="T56" s="19">
         <f>IF($K56,ABS(_xll.RtGet(SourceAlias,$L56,Q$2)-Q56),0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="U56" s="19" t="e">
+        <v>0.14642655614995026</v>
+      </c>
+      <c r="U56" s="19">
         <f>IF($K56,ABS(_xll.RtGet(SourceAlias,$L56,R$2)-R56),0)</f>
-        <v>#NUM!</v>
+        <v>0.14642655614995026</v>
       </c>
     </row>
     <row r="57" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6323,32 +6328,32 @@
       <c r="M57" s="5"/>
       <c r="N57" s="5">
         <f t="shared" si="3"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O57" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B57,J57,Currency,Calendar,E57,"mf",F57,H57,$F$38,,Trigger)</f>
-        <v>obj_00189#0000</v>
+        <v>obj_001b2#0000</v>
       </c>
       <c r="P57" s="5"/>
-      <c r="Q57" s="19" t="e">
+      <c r="Q57" s="19">
         <f>_xll.qlIndexFixing(O57,N57,,TriggerCounter)*100</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R57" s="19" t="e">
+        <v>1.2976306753664633</v>
+      </c>
+      <c r="R57" s="19">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>1.2976306753664633</v>
       </c>
       <c r="S57" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K57),_xll.RtContribute(SourceAlias,$L57,Fields,Q57:R57,"SCOPE:SERVER"),"--")</f>
         <v>--</v>
       </c>
-      <c r="T57" s="19" t="e">
+      <c r="T57" s="19">
         <f>IF($K57,ABS(_xll.RtGet(SourceAlias,$L57,Q$2)-Q57),0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="U57" s="19" t="e">
+        <v>0.16318707036646329</v>
+      </c>
+      <c r="U57" s="19">
         <f>IF($K57,ABS(_xll.RtGet(SourceAlias,$L57,R$2)-R57),0)</f>
-        <v>#NUM!</v>
+        <v>0.16318707036646329</v>
       </c>
     </row>
     <row r="58" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6388,32 +6393,32 @@
       <c r="M58" s="5"/>
       <c r="N58" s="5">
         <f t="shared" si="3"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O58" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B58,J58,Currency,Calendar,E58,"mf",F58,H58,$F$38,,Trigger)</f>
-        <v>obj_00197#0000</v>
+        <v>obj_001a4#0000</v>
       </c>
       <c r="P58" s="5"/>
-      <c r="Q58" s="19" t="e">
+      <c r="Q58" s="19">
         <f>_xll.qlIndexFixing(O58,N58,,TriggerCounter)*100</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R58" s="19" t="e">
+        <v>1.3592537039821611</v>
+      </c>
+      <c r="R58" s="19">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>1.3592537039821611</v>
       </c>
       <c r="S58" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K58),_xll.RtContribute(SourceAlias,$L58,Fields,Q58:R58,"SCOPE:SERVER"),"--")</f>
         <v>--</v>
       </c>
-      <c r="T58" s="19" t="e">
+      <c r="T58" s="19">
         <f>IF($K58,ABS(_xll.RtGet(SourceAlias,$L58,Q$2)-Q58),0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="U58" s="19" t="e">
+        <v>0.17315389798216096</v>
+      </c>
+      <c r="U58" s="19">
         <f>IF($K58,ABS(_xll.RtGet(SourceAlias,$L58,R$2)-R58),0)</f>
-        <v>#NUM!</v>
+        <v>0.17315389798216096</v>
       </c>
     </row>
     <row r="59" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6453,32 +6458,32 @@
       <c r="M59" s="5"/>
       <c r="N59" s="5">
         <f t="shared" si="3"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O59" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B59,J59,Currency,Calendar,E59,"mf",F59,H59,$F$38,,Trigger)</f>
-        <v>obj_00186#0000</v>
+        <v>obj_001ad#0000</v>
       </c>
       <c r="P59" s="5"/>
-      <c r="Q59" s="19" t="e">
+      <c r="Q59" s="19">
         <f>_xll.qlIndexFixing(O59,N59,,TriggerCounter)*100</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R59" s="19" t="e">
+        <v>1.4299596067124603</v>
+      </c>
+      <c r="R59" s="19">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>1.4299596067124603</v>
       </c>
       <c r="S59" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K59),_xll.RtContribute(SourceAlias,$L59,Fields,Q59:R59,"SCOPE:SERVER"),"--")</f>
         <v>--</v>
       </c>
-      <c r="T59" s="19" t="e">
+      <c r="T59" s="19">
         <f>IF($K59,ABS(_xll.RtGet(SourceAlias,$L59,Q$2)-Q59),0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="U59" s="19" t="e">
+        <v>0.18478709171246033</v>
+      </c>
+      <c r="U59" s="19">
         <f>IF($K59,ABS(_xll.RtGet(SourceAlias,$L59,R$2)-R59),0)</f>
-        <v>#NUM!</v>
+        <v>0.18478709171246033</v>
       </c>
     </row>
     <row r="60" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6518,32 +6523,32 @@
       <c r="M60" s="5"/>
       <c r="N60" s="5">
         <f t="shared" si="3"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O60" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B60,J60,Currency,Calendar,E60,"mf",F60,H60,$F$38,,Trigger)</f>
-        <v>obj_0019b#0000</v>
+        <v>obj_001a1#0000</v>
       </c>
       <c r="P60" s="5"/>
-      <c r="Q60" s="19" t="e">
+      <c r="Q60" s="19">
         <f>_xll.qlIndexFixing(O60,N60,,TriggerCounter)*100</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R60" s="19" t="e">
+        <v>1.482885055553907</v>
+      </c>
+      <c r="R60" s="19">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>1.482885055553907</v>
       </c>
       <c r="S60" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K60),_xll.RtContribute(SourceAlias,$L60,Fields,Q60:R60,"SCOPE:SERVER"),"--")</f>
         <v>--</v>
       </c>
-      <c r="T60" s="19" t="e">
+      <c r="T60" s="19">
         <f>IF($K60,ABS(_xll.RtGet(SourceAlias,$L60,Q$2)-Q60),0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="U60" s="19" t="e">
+        <v>0.19348399755390711</v>
+      </c>
+      <c r="U60" s="19">
         <f>IF($K60,ABS(_xll.RtGet(SourceAlias,$L60,R$2)-R60),0)</f>
-        <v>#NUM!</v>
+        <v>0.19348399755390711</v>
       </c>
     </row>
     <row r="61" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6583,32 +6588,32 @@
       <c r="M61" s="5"/>
       <c r="N61" s="5">
         <f t="shared" si="3"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O61" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B61,J61,Currency,Calendar,E61,"mf",F61,H61,$F$38,,Trigger)</f>
-        <v>obj_0018d#0000</v>
+        <v>obj_001b4#0000</v>
       </c>
       <c r="P61" s="5"/>
-      <c r="Q61" s="19" t="e">
+      <c r="Q61" s="19">
         <f>_xll.qlIndexFixing(O61,N61,,TriggerCounter)*100</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R61" s="19" t="e">
+        <v>1.5034215549215684</v>
+      </c>
+      <c r="R61" s="19">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>1.5034215549215684</v>
       </c>
       <c r="S61" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K61),_xll.RtContribute(SourceAlias,$L61,Fields,Q61:R61,"SCOPE:SERVER"),"--")</f>
         <v>--</v>
       </c>
-      <c r="T61" s="19" t="e">
+      <c r="T61" s="19">
         <f>IF($K61,ABS(_xll.RtGet(SourceAlias,$L61,Q$2)-Q61),0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="U61" s="19" t="e">
+        <v>0.19685319492156839</v>
+      </c>
+      <c r="U61" s="19">
         <f>IF($K61,ABS(_xll.RtGet(SourceAlias,$L61,R$2)-R61),0)</f>
-        <v>#NUM!</v>
+        <v>0.19685319492156839</v>
       </c>
     </row>
     <row r="62" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6648,32 +6653,32 @@
       <c r="M62" s="5"/>
       <c r="N62" s="5">
         <f t="shared" si="3"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O62" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B62,J62,Currency,Calendar,E62,"mf",F62,H62,$F$38,,Trigger)</f>
-        <v>obj_00185#0000</v>
+        <v>obj_001b0#0000</v>
       </c>
       <c r="P62" s="5"/>
-      <c r="Q62" s="19" t="e">
+      <c r="Q62" s="19">
         <f>_xll.qlIndexFixing(O62,N62,,TriggerCounter)*100</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R62" s="19" t="e">
+        <v>1.5239658882240654</v>
+      </c>
+      <c r="R62" s="19">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>1.5239658882240654</v>
       </c>
       <c r="S62" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K62),_xll.RtContribute(SourceAlias,$L62,Fields,Q62:R62,"SCOPE:SERVER"),"--")</f>
         <v>--</v>
       </c>
-      <c r="T62" s="19" t="e">
+      <c r="T62" s="19">
         <f>IF($K62,ABS(_xll.RtGet(SourceAlias,$L62,Q$2)-Q62),0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="U62" s="19" t="e">
+        <v>0.20023113322406538</v>
+      </c>
+      <c r="U62" s="19">
         <f>IF($K62,ABS(_xll.RtGet(SourceAlias,$L62,R$2)-R62),0)</f>
-        <v>#NUM!</v>
+        <v>0.20023113322406538</v>
       </c>
     </row>
     <row r="63" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6741,19 +6746,19 @@
       <c r="N64" s="5"/>
       <c r="O64" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J64)</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="P64" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O64,"1d",,TRUE)</f>
-        <v>41737</v>
+        <v>41919</v>
       </c>
       <c r="Q64" s="19">
         <f>(_xll.qlYieldTSDiscount($F$63,O64,TriggerCounter)/_xll.qlYieldTSDiscount($F$63,P64)-1)/_xll.qlDayCounterYearFraction(F64,O64,P64)*100</f>
-        <v>0.20670861808913532</v>
+        <v>0.23872454994700032</v>
       </c>
       <c r="R64" s="19">
         <f t="shared" si="1"/>
-        <v>0.20670861808913532</v>
+        <v>0.23872454994700032</v>
       </c>
       <c r="S64" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K64),_xll.RtContribute(SourceAlias,$L64,Fields,Q64:R64,"SCOPE:SERVER"),"--")</f>
@@ -6761,11 +6766,11 @@
       </c>
       <c r="T64" s="19">
         <f>IF($K64,ABS(_xll.RtGet(SourceAlias,$L64,Q$2)-Q64),0)</f>
-        <v>6.9006659108646895E-3</v>
+        <v>5.2999687971677645E-11</v>
       </c>
       <c r="U64" s="19">
         <f>IF($K64,ABS(_xll.RtGet(SourceAlias,$L64,R$2)-R64),0)</f>
-        <v>6.9006659108646895E-3</v>
+        <v>5.2999687971677645E-11</v>
       </c>
     </row>
     <row r="65" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6806,19 +6811,19 @@
       <c r="N65" s="5"/>
       <c r="O65" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J65)</f>
-        <v>41738</v>
+        <v>41920</v>
       </c>
       <c r="P65" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O65,"1d",,TRUE)</f>
-        <v>41739</v>
+        <v>41921</v>
       </c>
       <c r="Q65" s="19">
         <f>(_xll.qlYieldTSDiscount($F$63,O65,TriggerCounter)/_xll.qlYieldTSDiscount($F$63,P65)-1)/_xll.qlDayCounterYearFraction(F65,O65,P65)*100</f>
-        <v>0.20668828696501773</v>
+        <v>0.23857555421313847</v>
       </c>
       <c r="R65" s="19">
         <f t="shared" si="1"/>
-        <v>0.20668828696501773</v>
+        <v>0.23857555421313847</v>
       </c>
       <c r="S65" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K65),_xll.RtContribute(SourceAlias,$L65,Fields,Q65:R65,"SCOPE:SERVER"),"--")</f>
@@ -6826,11 +6831,11 @@
       </c>
       <c r="T65" s="19">
         <f>IF($K65,ABS(_xll.RtGet(SourceAlias,$L65,Q$2)-Q65),0)</f>
-        <v>6.8770080349822571E-3</v>
+        <v>2.1313847908821515E-10</v>
       </c>
       <c r="U65" s="19">
         <f>IF($K65,ABS(_xll.RtGet(SourceAlias,$L65,R$2)-R65),0)</f>
-        <v>6.8770080349822571E-3</v>
+        <v>2.1313847908821515E-10</v>
       </c>
     </row>
     <row r="66" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6871,19 +6876,19 @@
       <c r="N66" s="5"/>
       <c r="O66" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J66)</f>
-        <v>41738</v>
+        <v>41920</v>
       </c>
       <c r="P66" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O66,"1d",,TRUE)</f>
-        <v>41739</v>
+        <v>41921</v>
       </c>
       <c r="Q66" s="19">
         <f>(_xll.qlYieldTSDiscount($F$63,O66,TriggerCounter)/_xll.qlYieldTSDiscount($F$63,P66)-1)/_xll.qlDayCounterYearFraction(F66,O66,P66)*100</f>
-        <v>0.20668828696501773</v>
+        <v>0.23857555421313847</v>
       </c>
       <c r="R66" s="19">
         <f t="shared" si="1"/>
-        <v>0.20668828696501773</v>
+        <v>0.23857555421313847</v>
       </c>
       <c r="S66" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K66),_xll.RtContribute(SourceAlias,$L66,Fields,Q66:R66,"SCOPE:SERVER"),"--")</f>
@@ -6891,11 +6896,11 @@
       </c>
       <c r="T66" s="19">
         <f>IF($K66,ABS(_xll.RtGet(SourceAlias,$L66,Q$2)-Q66),0)</f>
-        <v>6.8770080349822571E-3</v>
+        <v>2.1313847908821515E-10</v>
       </c>
       <c r="U66" s="19">
         <f>IF($K66,ABS(_xll.RtGet(SourceAlias,$L66,R$2)-R66),0)</f>
-        <v>6.8770080349822571E-3</v>
+        <v>2.1313847908821515E-10</v>
       </c>
     </row>
     <row r="67" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6936,19 +6941,19 @@
       <c r="N67" s="5"/>
       <c r="O67" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,J67)</f>
-        <v>41738</v>
+        <v>41920</v>
       </c>
       <c r="P67" s="5">
         <f>_xll.qlCalendarAdvance(Calendar,O67,"1d",,TRUE)</f>
-        <v>41739</v>
+        <v>41921</v>
       </c>
       <c r="Q67" s="19">
         <f>(_xll.qlYieldTSDiscount($F$63,O67,TriggerCounter)/_xll.qlYieldTSDiscount($F$63,P67)-1)/_xll.qlDayCounterYearFraction(F67,O67,P67)*100</f>
-        <v>0.20668828696501773</v>
+        <v>0.23857555421313847</v>
       </c>
       <c r="R67" s="19">
         <f t="shared" si="1"/>
-        <v>0.20668828696501773</v>
+        <v>0.23857555421313847</v>
       </c>
       <c r="S67" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K67),_xll.RtContribute(SourceAlias,$L67,Fields,Q67:R67,"SCOPE:SERVER"),"--")</f>
@@ -6956,11 +6961,11 @@
       </c>
       <c r="T67" s="19">
         <f>IF($K67,ABS(_xll.RtGet(SourceAlias,$L67,Q$2)-Q67),0)</f>
-        <v>6.8770080349822571E-3</v>
+        <v>2.1313847908821515E-10</v>
       </c>
       <c r="U67" s="19">
         <f>IF($K67,ABS(_xll.RtGet(SourceAlias,$L67,R$2)-R67),0)</f>
-        <v>6.8770080349822571E-3</v>
+        <v>2.1313847908821515E-10</v>
       </c>
     </row>
     <row r="68" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7000,20 +7005,20 @@
       <c r="M68" s="5"/>
       <c r="N68" s="5">
         <f t="shared" ref="N68:N79" si="4">EvaluationDate</f>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O68" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B68,J68,Currency,Calendar,E68,"mf",F68,H68,$F$19,,Trigger)</f>
-        <v>obj_00183#0000</v>
+        <v>obj_001a5#0000</v>
       </c>
       <c r="P68" s="5"/>
       <c r="Q68" s="19">
         <f>_xll.qlIndexFixing(O68,N68,,TriggerCounter)*100</f>
-        <v>0.21002997749571756</v>
+        <v>0.21003262646422413</v>
       </c>
       <c r="R68" s="19">
         <f t="shared" si="1"/>
-        <v>0.21002997749571756</v>
+        <v>0.21003262646422413</v>
       </c>
       <c r="S68" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K68),_xll.RtContribute(SourceAlias,$L68,Fields,Q68:R68,"SCOPE:SERVER"),"--")</f>
@@ -7021,11 +7026,11 @@
       </c>
       <c r="T68" s="19">
         <f>IF($K68,ABS(_xll.RtGet(SourceAlias,$L68,Q$2)-Q68),0)</f>
-        <v>2.044504282455728E-6</v>
+        <v>2.0453577587176142E-7</v>
       </c>
       <c r="U68" s="19">
         <f>IF($K68,ABS(_xll.RtGet(SourceAlias,$L68,R$2)-R68),0)</f>
-        <v>2.044504282455728E-6</v>
+        <v>2.0453577587176142E-7</v>
       </c>
     </row>
     <row r="69" spans="2:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7065,20 +7070,20 @@
       <c r="M69" s="5"/>
       <c r="N69" s="5">
         <f t="shared" si="4"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O69" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B69,J69,Currency,Calendar,E69,"mf",F69,H69,$F$19,,Trigger)</f>
-        <v>obj_0018b#0000</v>
+        <v>obj_001af#0000</v>
       </c>
       <c r="P69" s="5"/>
       <c r="Q69" s="19">
         <f>_xll.qlIndexFixing(O69,N69,,TriggerCounter)*100</f>
-        <v>0.24006510373795428</v>
+        <v>0.23008005296315046</v>
       </c>
       <c r="R69" s="19">
         <f t="shared" si="1"/>
-        <v>0.24006510373795428</v>
+        <v>0.23008005296315046</v>
       </c>
       <c r="S69" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K69),_xll.RtContribute(SourceAlias,$L69,Fields,Q69:R69,"SCOPE:SERVER"),"--")</f>
@@ -7086,11 +7091,11 @@
       </c>
       <c r="T69" s="19">
         <f>IF($K69,ABS(_xll.RtGet(SourceAlias,$L69,Q$2)-Q69),0)</f>
-        <v>6.45226204570859E-6</v>
+        <v>5.7903684955173951E-7</v>
       </c>
       <c r="U69" s="19">
         <f>IF($K69,ABS(_xll.RtGet(SourceAlias,$L69,R$2)-R69),0)</f>
-        <v>6.45226204570859E-6</v>
+        <v>5.7903684955173951E-7</v>
       </c>
     </row>
     <row r="70" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7130,20 +7135,20 @@
       <c r="M70" s="5"/>
       <c r="N70" s="5">
         <f t="shared" si="4"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O70" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B70,J70,Currency,Calendar,E70,"mf",F70,H70,$F$19,,Trigger)</f>
-        <v>obj_00196#0000</v>
+        <v>obj_001aa#0000</v>
       </c>
       <c r="P70" s="5"/>
       <c r="Q70" s="19">
         <f>_xll.qlIndexFixing(O70,N70,,TriggerCounter)*100</f>
-        <v>0.2601196702397961</v>
+        <v>0.25013003129926648</v>
       </c>
       <c r="R70" s="19">
         <f t="shared" si="1"/>
-        <v>0.2601196702397961</v>
+        <v>0.25013003129926648</v>
       </c>
       <c r="S70" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K70),_xll.RtContribute(SourceAlias,$L70,Fields,Q70:R70,"SCOPE:SERVER"),"--")</f>
@@ -7151,11 +7156,11 @@
       </c>
       <c r="T70" s="19">
         <f>IF($K70,ABS(_xll.RtGet(SourceAlias,$L70,Q$2)-Q70),0)</f>
-        <v>9.9964787602039307E-3</v>
+        <v>5.432992664644587E-7</v>
       </c>
       <c r="U70" s="19">
         <f>IF($K70,ABS(_xll.RtGet(SourceAlias,$L70,R$2)-R70),0)</f>
-        <v>9.9964787602039307E-3</v>
+        <v>5.432992664644587E-7</v>
       </c>
     </row>
     <row r="71" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7195,20 +7200,20 @@
       <c r="M71" s="5"/>
       <c r="N71" s="5">
         <f t="shared" si="4"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O71" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B71,J71,Currency,Calendar,E71,"mf",F71,H71,$F$19,,Trigger)</f>
-        <v>obj_00191#0000</v>
+        <v>obj_001a7#0000</v>
       </c>
       <c r="P71" s="5"/>
       <c r="Q71" s="19">
         <f>_xll.qlIndexFixing(O71,N71,,TriggerCounter)*100</f>
-        <v>0.2901753686155864</v>
+        <v>0.34012232117100916</v>
       </c>
       <c r="R71" s="19">
         <f t="shared" si="1"/>
-        <v>0.2901753686155864</v>
+        <v>0.34012232117100916</v>
       </c>
       <c r="S71" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K71),_xll.RtContribute(SourceAlias,$L71,Fields,Q71:R71,"SCOPE:SERVER"),"--")</f>
@@ -7216,15 +7221,15 @@
       </c>
       <c r="T71" s="19">
         <f>IF($K71,ABS(_xll.RtGet(SourceAlias,$L71,Q$2)-Q71),0)</f>
-        <v>9.9997233844135724E-3</v>
+        <v>1.2223171009129175E-5</v>
       </c>
       <c r="U71" s="19">
         <f>IF($K71,ABS(_xll.RtGet(SourceAlias,$L71,R$2)-R71),0)</f>
-        <v>9.9997233844135724E-3</v>
+        <v>1.2223171009129175E-5</v>
       </c>
     </row>
     <row r="72" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="21" t="s">
+      <c r="B72" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C72" s="21" t="s">
@@ -7254,17 +7259,17 @@
       <c r="K72" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="L72" s="42" t="s">
+      <c r="L72" s="39" t="s">
         <v>98</v>
       </c>
       <c r="M72" s="5"/>
       <c r="N72" s="5">
         <f t="shared" si="4"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O72" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B72,J72,Currency,Calendar,E72,"mf",F72,H72,$F$19,,Trigger)</f>
-        <v>obj_0018f#0000</v>
+        <v>obj_001a8#0000</v>
       </c>
       <c r="P72" s="5"/>
       <c r="Q72" s="19" t="e">
@@ -7289,7 +7294,7 @@
       </c>
     </row>
     <row r="73" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="21" t="s">
+      <c r="B73" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C73" s="21" t="s">
@@ -7319,17 +7324,17 @@
       <c r="K73" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="L73" s="42" t="s">
+      <c r="L73" s="39" t="s">
         <v>99</v>
       </c>
       <c r="M73" s="5"/>
       <c r="N73" s="5">
         <f t="shared" si="4"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O73" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B73,J73,Currency,Calendar,E73,"mf",F73,H73,$F$19,,Trigger)</f>
-        <v>obj_00192#0000</v>
+        <v>obj_001ac#0000</v>
       </c>
       <c r="P73" s="5"/>
       <c r="Q73" s="19" t="e">
@@ -7390,11 +7395,11 @@
       <c r="M74" s="5"/>
       <c r="N74" s="5">
         <f t="shared" si="4"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O74" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B74,J74,Currency,Calendar,E74,"mf",F74,H74,$F$19,,Trigger)</f>
-        <v>obj_0018e#0000</v>
+        <v>obj_001a3#0000</v>
       </c>
       <c r="P74" s="5"/>
       <c r="Q74" s="19" t="e">
@@ -7455,11 +7460,11 @@
       <c r="M75" s="5"/>
       <c r="N75" s="5">
         <f t="shared" si="4"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O75" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B75,J75,Currency,Calendar,E75,"mf",F75,H75,$F$19,,Trigger)</f>
-        <v>obj_0019a#0000</v>
+        <v>obj_001ae#0000</v>
       </c>
       <c r="P75" s="5"/>
       <c r="Q75" s="19" t="e">
@@ -7520,11 +7525,11 @@
       <c r="M76" s="5"/>
       <c r="N76" s="5">
         <f t="shared" si="4"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O76" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B76,J76,Currency,Calendar,E76,"mf",F76,H76,$F$19,,Trigger)</f>
-        <v>obj_00193#0000</v>
+        <v>obj_001b3#0000</v>
       </c>
       <c r="P76" s="5"/>
       <c r="Q76" s="19" t="e">
@@ -7585,11 +7590,11 @@
       <c r="M77" s="5"/>
       <c r="N77" s="5">
         <f t="shared" si="4"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O77" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B77,J77,Currency,Calendar,E77,"mf",F77,H77,$F$19,,Trigger)</f>
-        <v>obj_00194#0000</v>
+        <v>obj_001b7#0000</v>
       </c>
       <c r="P77" s="5"/>
       <c r="Q77" s="19" t="e">
@@ -7650,11 +7655,11 @@
       <c r="M78" s="5"/>
       <c r="N78" s="5">
         <f t="shared" si="4"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O78" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B78,J78,Currency,Calendar,E78,"mf",F78,H78,$F$19,,Trigger)</f>
-        <v>obj_00190#0000</v>
+        <v>obj_001a0#0000</v>
       </c>
       <c r="P78" s="5"/>
       <c r="Q78" s="19" t="e">
@@ -7715,11 +7720,11 @@
       <c r="M79" s="5"/>
       <c r="N79" s="5">
         <f t="shared" si="4"/>
-        <v>41736</v>
+        <v>41918</v>
       </c>
       <c r="O79" s="5" t="str">
         <f>_xll.qlSwapIndex(,,B79,J79,Currency,Calendar,E79,"mf",F79,H79,$F$19,,Trigger)</f>
-        <v>obj_0019d#0000</v>
+        <v>obj_001a2#0000</v>
       </c>
       <c r="P79" s="5"/>
       <c r="Q79" s="19" t="e">
@@ -7810,11 +7815,11 @@
       <c r="P81" s="5"/>
       <c r="Q81" s="19">
         <f>[1]OIS!$Q$8</f>
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="R81" s="19">
         <f t="shared" si="1"/>
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="S81" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K81),_xll.RtContribute(SourceAlias,$L81,Fields,Q81:R81,"SCOPE:SERVER"),"--")</f>
@@ -7822,11 +7827,11 @@
       </c>
       <c r="T81" s="19">
         <f>IF($K81,ABS(_xll.RtGet(SourceAlias,$L81,Q$2)-Q81),0)</f>
-        <v>0</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="U81" s="19">
         <f>IF($K81,ABS(_xll.RtGet(SourceAlias,$L81,R$2)-R81),0)</f>
-        <v>0</v>
+        <v>9.999999999999995E-3</v>
       </c>
     </row>
     <row r="82" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7869,11 +7874,11 @@
       <c r="P82" s="5"/>
       <c r="Q82" s="19">
         <f>[1]OIS!$Q$9</f>
-        <v>6.9999999999999993E-2</v>
+        <v>0.06</v>
       </c>
       <c r="R82" s="19">
         <f t="shared" si="1"/>
-        <v>6.9999999999999993E-2</v>
+        <v>0.06</v>
       </c>
       <c r="S82" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K82),_xll.RtContribute(SourceAlias,$L82,Fields,Q82:R82,"SCOPE:SERVER"),"--")</f>
@@ -7881,11 +7886,11 @@
       </c>
       <c r="T82" s="19">
         <f>IF($K82,ABS(_xll.RtGet(SourceAlias,$L82,Q$2)-Q82),0)</f>
-        <v>1.3877787807814457E-17</v>
+        <v>1.0000000000000009E-2</v>
       </c>
       <c r="U82" s="19">
         <f>IF($K82,ABS(_xll.RtGet(SourceAlias,$L82,R$2)-R82),0)</f>
-        <v>1.3877787807814457E-17</v>
+        <v>1.0000000000000009E-2</v>
       </c>
     </row>
     <row r="83" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7928,11 +7933,11 @@
       <c r="P83" s="5"/>
       <c r="Q83" s="19">
         <f>[1]OIS!$Q$10</f>
-        <v>9.0000000000000011E-2</v>
+        <v>6.9999999999999993E-2</v>
       </c>
       <c r="R83" s="19">
         <f t="shared" si="1"/>
-        <v>9.0000000000000011E-2</v>
+        <v>6.9999999999999993E-2</v>
       </c>
       <c r="S83" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K83),_xll.RtContribute(SourceAlias,$L83,Fields,Q83:R83,"SCOPE:SERVER"),"--")</f>
@@ -7940,11 +7945,11 @@
       </c>
       <c r="T83" s="19">
         <f>IF($K83,ABS(_xll.RtGet(SourceAlias,$L83,Q$2)-Q83),0)</f>
-        <v>1.3877787807814457E-17</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="U83" s="19">
         <f>IF($K83,ABS(_xll.RtGet(SourceAlias,$L83,R$2)-R83),0)</f>
-        <v>1.3877787807814457E-17</v>
+        <v>2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="84" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7987,11 +7992,11 @@
       <c r="P84" s="5"/>
       <c r="Q84" s="19">
         <f>[1]OIS!$Q$11</f>
-        <v>0.12000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="R84" s="19">
         <f t="shared" ref="R84:R97" si="5">Q84</f>
-        <v>0.12000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="S84" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K84),_xll.RtContribute(SourceAlias,$L84,Fields,Q84:R84,"SCOPE:SERVER"),"--")</f>
@@ -7999,11 +8004,11 @@
       </c>
       <c r="T84" s="19">
         <f>IF($K84,ABS(_xll.RtGet(SourceAlias,$L84,Q$2)-Q84),0)</f>
-        <v>1.3877787807814457E-17</v>
+        <v>1.999999999999999E-2</v>
       </c>
       <c r="U84" s="19">
         <f>IF($K84,ABS(_xll.RtGet(SourceAlias,$L84,R$2)-R84),0)</f>
-        <v>1.3877787807814457E-17</v>
+        <v>1.999999999999999E-2</v>
       </c>
     </row>
     <row r="85" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8046,11 +8051,11 @@
       <c r="P85" s="5"/>
       <c r="Q85" s="19">
         <f>[1]OIS!$Q$12</f>
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="R85" s="19">
         <f t="shared" si="5"/>
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="S85" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K85),_xll.RtContribute(SourceAlias,$L85,Fields,Q85:R85,"SCOPE:SERVER"),"--")</f>
@@ -8058,11 +8063,11 @@
       </c>
       <c r="T85" s="19">
         <f>IF($K85,ABS(_xll.RtGet(SourceAlias,$L85,Q$2)-Q85),0)</f>
-        <v>0</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="U85" s="19">
         <f>IF($K85,ABS(_xll.RtGet(SourceAlias,$L85,R$2)-R85),0)</f>
-        <v>0</v>
+        <v>9.999999999999995E-3</v>
       </c>
     </row>
     <row r="86" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8105,11 +8110,11 @@
       <c r="P86" s="5"/>
       <c r="Q86" s="19">
         <f>[1]OIS!$Q$13</f>
-        <v>0.11</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="R86" s="19">
         <f t="shared" si="5"/>
-        <v>0.11</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="S86" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K86),_xll.RtContribute(SourceAlias,$L86,Fields,Q86:R86,"SCOPE:SERVER"),"--")</f>
@@ -8117,11 +8122,11 @@
       </c>
       <c r="T86" s="19">
         <f>IF($K86,ABS(_xll.RtGet(SourceAlias,$L86,Q$2)-Q86),0)</f>
-        <v>0</v>
+        <v>1.0000000000000009E-2</v>
       </c>
       <c r="U86" s="19">
         <f>IF($K86,ABS(_xll.RtGet(SourceAlias,$L86,R$2)-R86),0)</f>
-        <v>0</v>
+        <v>1.0000000000000009E-2</v>
       </c>
     </row>
     <row r="87" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8164,11 +8169,11 @@
       <c r="P87" s="5"/>
       <c r="Q87" s="19">
         <f>[1]OIS!$Q$16</f>
-        <v>0.16999999999999998</v>
+        <v>0.13</v>
       </c>
       <c r="R87" s="19">
         <f t="shared" si="5"/>
-        <v>0.16999999999999998</v>
+        <v>0.13</v>
       </c>
       <c r="S87" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K87),_xll.RtContribute(SourceAlias,$L87,Fields,Q87:R87,"SCOPE:SERVER"),"--")</f>
@@ -8176,11 +8181,11 @@
       </c>
       <c r="T87" s="19">
         <f>IF($K87,ABS(_xll.RtGet(SourceAlias,$L87,Q$2)-Q87),0)</f>
-        <v>2.7755575615628914E-17</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="U87" s="19">
         <f>IF($K87,ABS(_xll.RtGet(SourceAlias,$L87,R$2)-R87),0)</f>
-        <v>2.7755575615628914E-17</v>
+        <v>4.0000000000000008E-2</v>
       </c>
     </row>
     <row r="88" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8223,11 +8228,11 @@
       <c r="P88" s="5"/>
       <c r="Q88" s="19">
         <f>[1]OIS!$Q$19</f>
-        <v>0.2</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="R88" s="19">
         <f t="shared" si="5"/>
-        <v>0.2</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="S88" s="20" t="str">
         <f>IF(AND(UPPER(ContributionPassword)="ABCD",K88),_xll.RtContribute(SourceAlias,$L88,Fields,Q88:R88,"SCOPE:SERVER"),"--")</f>
@@ -8235,11 +8240,11 @@
       </c>
       <c r="T88" s="19">
         <f>IF($K88,ABS(_xll.RtGet(SourceAlias,$L88,Q$2)-Q88),0)</f>
-        <v>0</v>
+        <v>4.9999999999999989E-2</v>
       </c>
       <c r="U88" s="19">
         <f>IF($K88,ABS(_xll.RtGet(SourceAlias,$L88,R$2)-R88),0)</f>
-        <v>0</v>
+        <v>4.9999999999999989E-2</v>
       </c>
     </row>
     <row r="89" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
NEW HKD MX Contributor with correction
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_MxContributor.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_MxContributor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="19065" yWindow="-15" windowWidth="19110" windowHeight="11700" activeTab="1"/>
+    <workbookView xWindow="12705" yWindow="-15" windowWidth="12720" windowHeight="12105" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="2" r:id="rId1"/>
@@ -1255,8 +1255,6 @@
 HKD6M2X8F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AG16" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>0.48023117599999998</v>
         <stp/>
@@ -1308,8 +1306,6 @@
 HKD6M2X8F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AH16" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>0.83714</v>
         <stp/>
@@ -1347,8 +1343,6 @@
 HKD3M3X6F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AF14" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>0.36777256200000003</v>
         <stp/>
@@ -1377,8 +1371,6 @@
 HKDSTD1WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AK7" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>0.366750833</v>
         <stp/>
@@ -1906,8 +1898,6 @@
         <stp xml:space="preserve">	HKD3M3MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AE11" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>1.090377151</v>
         <stp/>
@@ -1976,8 +1966,6 @@
         <stp xml:space="preserve">	HKD1M2WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AC8" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>2.5</v>
         <stp/>
@@ -2011,6 +1999,8 @@
         <stp>_x0008_HKD6M7Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AG26" s="7"/>
       </tp>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>2.5</v>
         <stp/>
@@ -2033,8 +2023,6 @@
         <stp xml:space="preserve">	HKD3M18M=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AE21" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>2.29</v>
         <stp/>
@@ -2096,8 +2084,6 @@
         <stp>_x0008_HKD1M9M=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AC17" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>2.29</v>
         <stp/>
@@ -2158,6 +2144,8 @@
         <stp xml:space="preserve">	HKD3M18M=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AF21" s="7"/>
       </tp>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>2.29</v>
         <stp/>
@@ -2250,6 +2238,8 @@
         <stp xml:space="preserve">	HKD1M15Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AC29" s="7"/>
       </tp>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>0.22830397699999999</v>
         <stp/>
@@ -2292,6 +2282,8 @@
         <stp xml:space="preserve">	HKD6M15Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AG29" s="7"/>
       </tp>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>0.37797774699999998</v>
         <stp/>
@@ -2926,7 +2918,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="60">
-        <v>41922.536689814813</v>
+        <v>41922.576851851853</v>
       </c>
       <c r="E4" s="59"/>
       <c r="F4" s="2"/>
@@ -6847,8 +6839,8 @@
         <v>4.4526308334846831E-10</v>
       </c>
       <c r="AK9" s="89">
-        <f>ABS(_xll.RtGet(SourceAlias,$Y9,BID)-Z10)</f>
-        <v>8.7849999999999984E-2</v>
+        <f>ABS(_xll.RtGet(SourceAlias,$Y9,BID)-Z9)</f>
+        <v>0</v>
       </c>
       <c r="AL9" s="89">
         <f>ABS(_xll.RtGet(SourceAlias,$Y9,ASK)-AA9)</f>
@@ -6989,8 +6981,8 @@
         <v>1.0306847736396563E-10</v>
       </c>
       <c r="AK10" s="89">
-        <f>ABS(_xll.RtGet(SourceAlias,$Y10,BID)-Z11)</f>
-        <v>6.2930000000000041E-2</v>
+        <f>ABS(_xll.RtGet(SourceAlias,$Y10,BID)-Z10)</f>
+        <v>0</v>
       </c>
       <c r="AL10" s="89">
         <f>ABS(_xll.RtGet(SourceAlias,$Y10,ASK)-AA10)</f>
@@ -7169,8 +7161,8 @@
         <v>1.5819595633459471E-11</v>
       </c>
       <c r="AK11" s="89">
-        <f>ABS(_xll.RtGet(SourceAlias,$Y11,BID)-Z14)</f>
-        <v>0.16131000000000001</v>
+        <f>ABS(_xll.RtGet(SourceAlias,$Y11,BID)-Z11)</f>
+        <v>0</v>
       </c>
       <c r="AL11" s="89">
         <f>ABS(_xll.RtGet(SourceAlias,$Y11,ASK)-AA11)</f>
@@ -7612,8 +7604,8 @@
         <v>1.9345636204093353E-14</v>
       </c>
       <c r="AK14" s="89">
-        <f>ABS(_xll.RtGet(SourceAlias,$Y14,BID)-Z20)</f>
-        <v>0.30218999999999996</v>
+        <f>ABS(_xll.RtGet(SourceAlias,$Y14,BID)-Z14)</f>
+        <v>0</v>
       </c>
       <c r="AL14" s="89">
         <f>ABS(_xll.RtGet(SourceAlias,$Y14,ASK)-AA14)</f>
@@ -14201,7 +14193,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D7="ON",D7="TN",D7="SN"),"1D",IF(D7="SW","1W",D7)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001d2#0000</v>
+        <v>obj_001c8#0000</v>
       </c>
       <c r="N7" s="75"/>
       <c r="O7" s="79"/>
@@ -14251,7 +14243,7 @@
       <c r="L8" s="38"/>
       <c r="M8" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D8="ON",D8="TN",D8="SN"),"1D",IF(D8="SW","1W",D8)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001d8#0000</v>
+        <v>obj_001b6#0000</v>
       </c>
       <c r="N8" s="75"/>
       <c r="O8" s="79"/>
@@ -14301,7 +14293,7 @@
       <c r="L9" s="38"/>
       <c r="M9" s="108" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D9="ON",D9="TN",D9="SN"),"1D",IF(D9="SW","1W",D9)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00209#0000</v>
+        <v>obj_001da#0000</v>
       </c>
       <c r="N9" s="75"/>
       <c r="O9" s="79"/>
@@ -14387,7 +14379,7 @@
       <c r="L11" s="38"/>
       <c r="M11" s="78" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D11,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ec#0000</v>
+        <v>obj_001b9#0000</v>
       </c>
       <c r="N11" s="38"/>
       <c r="O11" s="77" t="s">
@@ -14440,7 +14432,7 @@
       <c r="L12" s="38"/>
       <c r="M12" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D12,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00201#0000</v>
+        <v>obj_001c0#0000</v>
       </c>
       <c r="N12" s="38"/>
       <c r="O12" s="79"/>
@@ -14487,7 +14479,7 @@
       <c r="L13" s="38"/>
       <c r="M13" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D13,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f0#0000</v>
+        <v>obj_001d0#0000</v>
       </c>
       <c r="N13" s="38"/>
       <c r="O13" s="79"/>
@@ -14537,7 +14529,7 @@
       <c r="L14" s="38"/>
       <c r="M14" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D14,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c9#0000</v>
+        <v>obj_001ec#0000</v>
       </c>
       <c r="N14" s="38"/>
       <c r="O14" s="79"/>
@@ -14584,7 +14576,7 @@
       <c r="L15" s="38"/>
       <c r="M15" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D15,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00203#0000</v>
+        <v>obj_001de#0000</v>
       </c>
       <c r="N15" s="38"/>
       <c r="O15" s="79"/>
@@ -14631,7 +14623,7 @@
       <c r="L16" s="38"/>
       <c r="M16" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D16,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f6#0000</v>
+        <v>obj_001f4#0000</v>
       </c>
       <c r="N16" s="38"/>
       <c r="O16" s="79"/>
@@ -14681,7 +14673,7 @@
       <c r="L17" s="38"/>
       <c r="M17" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D17,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f3#0000</v>
+        <v>obj_001e9#0000</v>
       </c>
       <c r="N17" s="75"/>
       <c r="O17" s="79"/>
@@ -14728,7 +14720,7 @@
       <c r="L18" s="38"/>
       <c r="M18" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D18,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001cd#0000</v>
+        <v>obj_001ce#0000</v>
       </c>
       <c r="N18" s="75"/>
       <c r="O18" s="79"/>
@@ -14775,7 +14767,7 @@
       <c r="L19" s="38"/>
       <c r="M19" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D19,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d1#0000</v>
+        <v>obj_001f5#0000</v>
       </c>
       <c r="N19" s="75"/>
       <c r="O19" s="79"/>
@@ -14825,7 +14817,7 @@
       <c r="L20" s="38"/>
       <c r="M20" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D20,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f1#0000</v>
+        <v>obj_00200#0000</v>
       </c>
       <c r="N20" s="75"/>
       <c r="O20" s="79"/>
@@ -14872,7 +14864,7 @@
       <c r="L21" s="116"/>
       <c r="M21" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D21,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00206#0000</v>
+        <v>obj_001e4#0000</v>
       </c>
       <c r="N21" s="75"/>
       <c r="O21" s="79"/>
@@ -14922,7 +14914,7 @@
       <c r="L22" s="116"/>
       <c r="M22" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D22,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d4#0000</v>
+        <v>obj_001d3#0000</v>
       </c>
       <c r="N22" s="75"/>
       <c r="O22" s="79"/>
@@ -14972,7 +14964,7 @@
       <c r="L23" s="116"/>
       <c r="M23" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ba#0000</v>
+        <v>obj_001cb#0000</v>
       </c>
       <c r="N23" s="75"/>
       <c r="O23" s="79"/>
@@ -15022,7 +15014,7 @@
       <c r="L24" s="116"/>
       <c r="M24" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001cc#0000</v>
+        <v>obj_001e5#0000</v>
       </c>
       <c r="N24" s="75"/>
       <c r="O24" s="79"/>
@@ -15072,7 +15064,7 @@
       <c r="L25" s="116"/>
       <c r="M25" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d5#0000</v>
+        <v>obj_001ca#0000</v>
       </c>
       <c r="N25" s="75"/>
       <c r="O25" s="79"/>
@@ -15122,7 +15114,7 @@
       <c r="L26" s="116"/>
       <c r="M26" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e9#0000</v>
+        <v>obj_001c2#0000</v>
       </c>
       <c r="N26" s="75"/>
       <c r="O26" s="79"/>
@@ -15172,7 +15164,7 @@
       <c r="L27" s="116"/>
       <c r="M27" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001db#0000</v>
+        <v>obj_001b8#0000</v>
       </c>
       <c r="N27" s="75"/>
       <c r="O27" s="79"/>
@@ -15222,7 +15214,7 @@
       <c r="L28" s="116"/>
       <c r="M28" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ee#0000</v>
+        <v>obj_001ea#0000</v>
       </c>
       <c r="N28" s="75"/>
       <c r="O28" s="79"/>
@@ -15272,7 +15264,7 @@
       <c r="L29" s="116"/>
       <c r="M29" s="126" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0020c#0000</v>
+        <v>obj_001c1#0000</v>
       </c>
       <c r="N29" s="75"/>
       <c r="O29" s="79"/>
@@ -18343,7 +18335,7 @@
       <c r="L6" s="38"/>
       <c r="M6" s="78" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D6="ON",D6="TN",D6="SN"),"1D",IF(D6="SW","1W",D6)),0,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001fe#0000</v>
+        <v>obj_001bf#0000</v>
       </c>
       <c r="N6" s="75"/>
       <c r="O6" s="77" t="b">
@@ -18399,7 +18391,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D7="ON",D7="TN",D7="SN"),"1D",IF(D7="SW","1W",D7)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001fa#0000</v>
+        <v>obj_00206#0000</v>
       </c>
       <c r="N7" s="75"/>
       <c r="O7" s="79"/>
@@ -18449,7 +18441,7 @@
       <c r="L8" s="38"/>
       <c r="M8" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D8="ON",D8="TN",D8="SN"),"1D",IF(D8="SW","1W",D8)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001fd#0000</v>
+        <v>obj_001c7#0000</v>
       </c>
       <c r="N8" s="75"/>
       <c r="O8" s="79"/>
@@ -18499,7 +18491,7 @@
       <c r="L9" s="38"/>
       <c r="M9" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D9="ON",D9="TN",D9="SN"),"1D",IF(D9="SW","1W",D9)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001e0#0000</v>
+        <v>obj_001d9#0000</v>
       </c>
       <c r="N9" s="75"/>
       <c r="O9" s="79"/>
@@ -18546,7 +18538,7 @@
       <c r="L10" s="38"/>
       <c r="M10" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D10="ON",D10="TN",D10="SN"),"1D",IF(D10="SW","1W",D10)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_0020a#0000</v>
+        <v>obj_001c5#0000</v>
       </c>
       <c r="N10" s="75"/>
       <c r="O10" s="79"/>
@@ -18596,7 +18588,7 @@
       <c r="L11" s="38"/>
       <c r="M11" s="29" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D11="ON",D11="TN",D11="SN"),"1D",IF(D11="SW","1W",D11)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001d9#0000</v>
+        <v>obj_001cc#0000</v>
       </c>
       <c r="N11" s="38"/>
       <c r="O11" s="79"/>
@@ -19047,7 +19039,7 @@
       <c r="L20" s="116"/>
       <c r="M20" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D20,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001fb#0000</v>
+        <v>obj_001ba#0000</v>
       </c>
       <c r="N20" s="75"/>
       <c r="O20" s="77" t="s">
@@ -19103,7 +19095,7 @@
       <c r="L21" s="116"/>
       <c r="M21" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D21,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00205#0000</v>
+        <v>obj_001b7#0000</v>
       </c>
       <c r="N21" s="75"/>
       <c r="O21" s="79"/>
@@ -19153,7 +19145,7 @@
       <c r="L22" s="116"/>
       <c r="M22" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D22,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ef#0000</v>
+        <v>obj_00203#0000</v>
       </c>
       <c r="N22" s="75"/>
       <c r="O22" s="79"/>
@@ -19203,7 +19195,7 @@
       <c r="L23" s="116"/>
       <c r="M23" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001dc#0000</v>
+        <v>obj_001d5#0000</v>
       </c>
       <c r="N23" s="75"/>
       <c r="O23" s="79"/>
@@ -19253,7 +19245,7 @@
       <c r="L24" s="116"/>
       <c r="M24" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00200#0000</v>
+        <v>obj_00205#0000</v>
       </c>
       <c r="N24" s="75"/>
       <c r="O24" s="79"/>
@@ -19303,7 +19295,7 @@
       <c r="L25" s="116"/>
       <c r="M25" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f5#0000</v>
+        <v>obj_001bd#0000</v>
       </c>
       <c r="N25" s="75"/>
       <c r="O25" s="79"/>
@@ -19353,7 +19345,7 @@
       <c r="L26" s="116"/>
       <c r="M26" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001da#0000</v>
+        <v>obj_001e3#0000</v>
       </c>
       <c r="N26" s="75"/>
       <c r="O26" s="79"/>
@@ -19403,7 +19395,7 @@
       <c r="L27" s="116"/>
       <c r="M27" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f8#0000</v>
+        <v>obj_001ee#0000</v>
       </c>
       <c r="N27" s="75"/>
       <c r="O27" s="79"/>
@@ -19453,7 +19445,7 @@
       <c r="L28" s="116"/>
       <c r="M28" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00204#0000</v>
+        <v>obj_001be#0000</v>
       </c>
       <c r="N28" s="75"/>
       <c r="O28" s="79"/>
@@ -22560,7 +22552,7 @@
       <c r="L6" s="38"/>
       <c r="M6" s="78" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D6="ON",D6="TN",D6="SN"),"1D",IF(D6="SW","1W",D6)),0,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001fc#0000</v>
+        <v>obj_001c3#0000</v>
       </c>
       <c r="N6" s="75"/>
       <c r="O6" s="77" t="b">
@@ -22616,7 +22608,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D7="ON",D7="TN",D7="SN"),"1D",IF(D7="SW","1W",D7)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001e7#0000</v>
+        <v>obj_001f3#0000</v>
       </c>
       <c r="N7" s="75"/>
       <c r="O7" s="79"/>
@@ -22666,7 +22658,7 @@
       <c r="L8" s="38"/>
       <c r="M8" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D8="ON",D8="TN",D8="SN"),"1D",IF(D8="SW","1W",D8)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00202#0000</v>
+        <v>obj_001f1#0000</v>
       </c>
       <c r="N8" s="75"/>
       <c r="O8" s="79"/>
@@ -22716,7 +22708,7 @@
       <c r="L9" s="38"/>
       <c r="M9" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D9="ON",D9="TN",D9="SN"),"1D",IF(D9="SW","1W",D9)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001e1#0000</v>
+        <v>obj_001f2#0000</v>
       </c>
       <c r="N9" s="75"/>
       <c r="O9" s="79"/>
@@ -22766,7 +22758,7 @@
       <c r="L10" s="38"/>
       <c r="M10" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D10="ON",D10="TN",D10="SN"),"1D",IF(D10="SW","1W",D10)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001c3#0000</v>
+        <v>obj_001f6#0000</v>
       </c>
       <c r="N10" s="75"/>
       <c r="O10" s="79"/>
@@ -22816,7 +22808,7 @@
       <c r="L11" s="38"/>
       <c r="M11" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D11="ON",D11="TN",D11="SN"),"1D",IF(D11="SW","1W",D11)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_0020b#0000</v>
+        <v>obj_001c6#0000</v>
       </c>
       <c r="N11" s="38"/>
       <c r="O11" s="79"/>
@@ -22866,7 +22858,7 @@
       <c r="L12" s="38"/>
       <c r="M12" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D12="ON",D12="TN",D12="SN"),"1D",IF(D12="SW","1W",D12)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001ff#0000</v>
+        <v>obj_001d8#0000</v>
       </c>
       <c r="N12" s="38"/>
       <c r="O12" s="79"/>
@@ -22916,7 +22908,7 @@
       <c r="L13" s="38"/>
       <c r="M13" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D13="ON",D13="TN",D13="SN"),"1D",IF(D13="SW","1W",D13)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001df#0000</v>
+        <v>obj_001e0#0000</v>
       </c>
       <c r="N13" s="38"/>
       <c r="O13" s="79"/>
@@ -22966,7 +22958,7 @@
       <c r="L14" s="38"/>
       <c r="M14" s="29" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D14="ON",D14="TN",D14="SN"),"1D",IF(D14="SW","1W",D14)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001d6#0000</v>
+        <v>obj_00207#0000</v>
       </c>
       <c r="N14" s="38"/>
       <c r="O14" s="79"/>
@@ -23432,7 +23424,7 @@
       <c r="L23" s="116"/>
       <c r="M23" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d3#0000</v>
+        <v>obj_001d4#0000</v>
       </c>
       <c r="N23" s="75"/>
       <c r="O23" s="77" t="s">
@@ -23488,7 +23480,7 @@
       <c r="L24" s="116"/>
       <c r="M24" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00207#0000</v>
+        <v>obj_001bc#0000</v>
       </c>
       <c r="N24" s="75"/>
       <c r="O24" s="79"/>
@@ -23538,7 +23530,7 @@
       <c r="L25" s="116"/>
       <c r="M25" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c8#0000</v>
+        <v>obj_001d2#0000</v>
       </c>
       <c r="N25" s="75"/>
       <c r="O25" s="79"/>
@@ -23588,7 +23580,7 @@
       <c r="L26" s="116"/>
       <c r="M26" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f9#0000</v>
+        <v>obj_001f7#0000</v>
       </c>
       <c r="N26" s="75"/>
       <c r="O26" s="79"/>
@@ -23638,7 +23630,7 @@
       <c r="L27" s="116"/>
       <c r="M27" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f4#0000</v>
+        <v>obj_001dc#0000</v>
       </c>
       <c r="N27" s="75"/>
       <c r="O27" s="79"/>
@@ -23688,7 +23680,7 @@
       <c r="L28" s="116"/>
       <c r="M28" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001bb#0000</v>
+        <v>obj_001fa#0000</v>
       </c>
       <c r="N28" s="75"/>
       <c r="O28" s="79"/>
@@ -23738,7 +23730,7 @@
       <c r="L29" s="116"/>
       <c r="M29" s="126" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e6#0000</v>
+        <v>obj_001ff#0000</v>
       </c>
       <c r="N29" s="75"/>
       <c r="O29" s="79"/>
@@ -26666,7 +26658,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="29" t="str">
         <f>_xll.qlOvernightIndex(,"Honix",0,Currency,Calendar,"act/365 (fixed)",YieldCurve,,Trigger)</f>
-        <v>obj_001bd#0000</v>
+        <v>obj_001cd#0000</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="79"/>
@@ -26791,7 +26783,7 @@
       <c r="L6" s="38"/>
       <c r="M6" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D6="ON","1D",D6),SettlementDays,Currency,Calendar,FixedLegTenor,"Following",FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ed#0000</v>
+        <v>obj_0020a#0000</v>
       </c>
       <c r="N6" s="75"/>
       <c r="O6" s="77" t="s">
@@ -26844,7 +26836,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D7="ON","1D",D7),SettlementDays,Currency,Calendar,FixedLegTenor,"Following",FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ea#0000</v>
+        <v>obj_0020b#0000</v>
       </c>
       <c r="N7" s="75"/>
       <c r="O7" s="79"/>
@@ -26891,7 +26883,7 @@
       <c r="L8" s="38"/>
       <c r="M8" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D8="ON","1D",D8),SettlementDays,Currency,Calendar,FixedLegTenor,"Following",FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d0#0000</v>
+        <v>obj_001e7#0000</v>
       </c>
       <c r="N8" s="75"/>
       <c r="O8" s="79"/>
@@ -26941,7 +26933,7 @@
       <c r="L9" s="38"/>
       <c r="M9" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D9="ON","1D",D9),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c2#0000</v>
+        <v>obj_00209#0000</v>
       </c>
       <c r="N9" s="75"/>
       <c r="O9" s="79"/>
@@ -26991,7 +26983,7 @@
       <c r="L10" s="38"/>
       <c r="M10" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D10="ON","1D",D10),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e3#0000</v>
+        <v>obj_001fb#0000</v>
       </c>
       <c r="N10" s="75"/>
       <c r="O10" s="79"/>
@@ -27041,7 +27033,7 @@
       <c r="L11" s="38"/>
       <c r="M11" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D11="ON","1D",D11),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c0#0000</v>
+        <v>obj_001fc#0000</v>
       </c>
       <c r="N11" s="75"/>
       <c r="O11" s="79"/>
@@ -27091,7 +27083,7 @@
       <c r="L12" s="38"/>
       <c r="M12" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D12="ON","1D",D12),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c1#0000</v>
+        <v>obj_00208#0000</v>
       </c>
       <c r="N12" s="75"/>
       <c r="O12" s="79"/>
@@ -27141,7 +27133,7 @@
       <c r="L13" s="38"/>
       <c r="M13" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D13="ON","1D",D13),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c6#0000</v>
+        <v>obj_00204#0000</v>
       </c>
       <c r="N13" s="75"/>
       <c r="O13" s="79"/>
@@ -27191,7 +27183,7 @@
       <c r="L14" s="38"/>
       <c r="M14" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D14="ON","1D",D14),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001bf#0000</v>
+        <v>obj_001f9#0000</v>
       </c>
       <c r="N14" s="75"/>
       <c r="O14" s="79"/>
@@ -27238,7 +27230,7 @@
       <c r="L15" s="38"/>
       <c r="M15" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D15="ON","1D",D15),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e2#0000</v>
+        <v>obj_001f0#0000</v>
       </c>
       <c r="N15" s="75"/>
       <c r="O15" s="79"/>
@@ -27285,7 +27277,7 @@
       <c r="L16" s="38"/>
       <c r="M16" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D16="ON","1D",D16),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001be#0000</v>
+        <v>obj_0020c#0000</v>
       </c>
       <c r="N16" s="75"/>
       <c r="O16" s="79"/>
@@ -27335,7 +27327,7 @@
       <c r="L17" s="38"/>
       <c r="M17" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D17="ON","1D",D17),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e4#0000</v>
+        <v>obj_001ef#0000</v>
       </c>
       <c r="N17" s="75"/>
       <c r="O17" s="79"/>
@@ -27382,7 +27374,7 @@
       <c r="L18" s="38"/>
       <c r="M18" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D18="ON","1D",D18),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c5#0000</v>
+        <v>obj_001e2#0000</v>
       </c>
       <c r="N18" s="75"/>
       <c r="O18" s="79"/>
@@ -27429,7 +27421,7 @@
       <c r="L19" s="38"/>
       <c r="M19" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D19="ON","1D",D19),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ca#0000</v>
+        <v>obj_001d7#0000</v>
       </c>
       <c r="N19" s="75"/>
       <c r="O19" s="79"/>
@@ -27479,7 +27471,7 @@
       <c r="L20" s="116"/>
       <c r="M20" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D20="ON","1D",D20),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001dd#0000</v>
+        <v>obj_001d1#0000</v>
       </c>
       <c r="N20" s="75"/>
       <c r="O20" s="79"/>
@@ -27529,7 +27521,7 @@
       <c r="L21" s="116"/>
       <c r="M21" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D21="ON","1D",D21),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e5#0000</v>
+        <v>obj_001df#0000</v>
       </c>
       <c r="N21" s="75"/>
       <c r="O21" s="79"/>
@@ -27579,7 +27571,7 @@
       <c r="L22" s="116"/>
       <c r="M22" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D22="ON","1D",D22),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c4#0000</v>
+        <v>obj_001f8#0000</v>
       </c>
       <c r="N22" s="75"/>
       <c r="O22" s="79"/>
@@ -27629,7 +27621,7 @@
       <c r="L23" s="116"/>
       <c r="M23" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D23="ON","1D",D23),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e8#0000</v>
+        <v>obj_00201#0000</v>
       </c>
       <c r="N23" s="75"/>
       <c r="O23" s="79"/>
@@ -27679,7 +27671,7 @@
       <c r="L24" s="116"/>
       <c r="M24" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D24="ON","1D",D24),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ce#0000</v>
+        <v>obj_001d6#0000</v>
       </c>
       <c r="N24" s="75"/>
       <c r="O24" s="79"/>
@@ -27729,7 +27721,7 @@
       <c r="L25" s="116"/>
       <c r="M25" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D25="ON","1D",D25),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00208#0000</v>
+        <v>obj_001e8#0000</v>
       </c>
       <c r="N25" s="75"/>
       <c r="O25" s="79"/>
@@ -27779,7 +27771,7 @@
       <c r="L26" s="116"/>
       <c r="M26" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D26="ON","1D",D26),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001eb#0000</v>
+        <v>obj_001db#0000</v>
       </c>
       <c r="N26" s="75"/>
       <c r="O26" s="79"/>
@@ -27829,7 +27821,7 @@
       <c r="L27" s="116"/>
       <c r="M27" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D27="ON","1D",D27),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001cb#0000</v>
+        <v>obj_001fe#0000</v>
       </c>
       <c r="N27" s="75"/>
       <c r="O27" s="79"/>
@@ -27879,7 +27871,7 @@
       <c r="L28" s="116"/>
       <c r="M28" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D28="ON","1D",D28),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d7#0000</v>
+        <v>obj_001ed#0000</v>
       </c>
       <c r="N28" s="75"/>
       <c r="O28" s="79"/>
@@ -27929,7 +27921,7 @@
       <c r="L29" s="116"/>
       <c r="M29" s="126" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D29="ON","1D",D29),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c7#0000</v>
+        <v>obj_001dd#0000</v>
       </c>
       <c r="N29" s="75"/>
       <c r="O29" s="79"/>
@@ -31447,7 +31439,7 @@
       <c r="L22" s="116"/>
       <c r="M22" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D22,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001de#0000</v>
+        <v>obj_001bb#0000</v>
       </c>
       <c r="N22" s="75"/>
       <c r="O22" s="77" t="s">
@@ -31503,7 +31495,7 @@
       <c r="L23" s="116"/>
       <c r="M23" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f2#0000</v>
+        <v>obj_00202#0000</v>
       </c>
       <c r="N23" s="75"/>
       <c r="O23" s="79"/>
@@ -31553,7 +31545,7 @@
       <c r="L24" s="116"/>
       <c r="M24" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001b6#0000</v>
+        <v>obj_001eb#0000</v>
       </c>
       <c r="N24" s="75"/>
       <c r="O24" s="79"/>
@@ -31603,7 +31595,7 @@
       <c r="L25" s="116"/>
       <c r="M25" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001b7#0000</v>
+        <v>obj_001c9#0000</v>
       </c>
       <c r="N25" s="75"/>
       <c r="O25" s="79"/>
@@ -31653,7 +31645,7 @@
       <c r="L26" s="116"/>
       <c r="M26" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001b8#0000</v>
+        <v>obj_001e1#0000</v>
       </c>
       <c r="N26" s="75"/>
       <c r="O26" s="79"/>
@@ -31703,7 +31695,7 @@
       <c r="L27" s="116"/>
       <c r="M27" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001b9#0000</v>
+        <v>obj_001c4#0000</v>
       </c>
       <c r="N27" s="75"/>
       <c r="O27" s="79"/>
@@ -31753,7 +31745,7 @@
       <c r="L28" s="116"/>
       <c r="M28" s="117" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001bc#0000</v>
+        <v>obj_001e6#0000</v>
       </c>
       <c r="N28" s="75"/>
       <c r="O28" s="79"/>
@@ -31803,7 +31795,7 @@
       <c r="L29" s="116"/>
       <c r="M29" s="126" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f7#0000</v>
+        <v>obj_001fd#0000</v>
       </c>
       <c r="N29" s="75"/>
       <c r="O29" s="79"/>

</xml_diff>